<commit_message>
Fixed previous commit, results were for level 9
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95FE3B5-13C9-4214-9402-C8ADC0C0A3AE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076FF7F8-5CD3-453B-9B5A-585B782A451D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="30">
   <si>
     <t>GVGAI level</t>
   </si>
@@ -89,6 +89,27 @@
   </si>
   <si>
     <t>With any planner</t>
+  </si>
+  <si>
+    <t>Replanning</t>
+  </si>
+  <si>
+    <t>MPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butteflies </t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Inconsistencias</t>
+  </si>
+  <si>
+    <t>Nº planificaciones</t>
+  </si>
+  <si>
+    <t>(Hasta pasarse el nivel, con Cocoon (multiplicación de mariposas))</t>
   </si>
 </sst>
 </file>
@@ -781,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH57"/>
+  <dimension ref="A1:AH69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,6 +2861,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
More results. Fixing VGDL in chipschallenge
The same object can't have simultaneously stepBack and killIfHasMore
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076FF7F8-5CD3-453B-9B5A-585B782A451D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FD1939-CB3C-4952-93DC-479FAD3CDF5A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v0" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="40">
   <si>
     <t>GVGAI level</t>
   </si>
@@ -111,6 +112,36 @@
   <si>
     <t>(Hasta pasarse el nivel, con Cocoon (multiplicación de mariposas))</t>
   </si>
+  <si>
+    <t>Any planner</t>
+  </si>
+  <si>
+    <t>Levels fully planned</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Solved within the replanning arquitecture</t>
+  </si>
+  <si>
+    <t>simpBould</t>
+  </si>
+  <si>
+    <t>chips</t>
+  </si>
+  <si>
+    <t>boulder</t>
+  </si>
+  <si>
+    <t>(times planner called)</t>
+  </si>
+  <si>
+    <t>-1 = Timeout</t>
+  </si>
+  <si>
+    <t>Agent victories only</t>
+  </si>
 </sst>
 </file>
 
@@ -140,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +211,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -443,6 +480,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,6 +541,85 @@
         <a:xfrm>
           <a:off x="9590942" y="139212"/>
           <a:ext cx="1853712" cy="827942"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Timeout:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> 15 min</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>21982</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>36634</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>293078</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{309B0E4F-A219-4DBB-846C-3419452911B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8044963" y="2322634"/>
+          <a:ext cx="1172307" cy="315058"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -804,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,4 +3035,2108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
+  <dimension ref="A1:Z68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="25" width="10.42578125" customWidth="1"/>
+    <col min="26" max="26" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="O1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="M3" s="4"/>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="48">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48">
+        <v>5</v>
+      </c>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48">
+        <v>1</v>
+      </c>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="M4" s="4"/>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="3">
+        <v>-1</v>
+      </c>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48">
+        <v>1</v>
+      </c>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="M5" s="4"/>
+      <c r="O5" s="1">
+        <v>2</v>
+      </c>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="M6" s="4"/>
+      <c r="O6" s="1">
+        <v>3</v>
+      </c>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="X6" s="48">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="48"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="M7" s="4"/>
+      <c r="O7" s="1">
+        <v>4</v>
+      </c>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48">
+        <v>3</v>
+      </c>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48">
+        <v>1</v>
+      </c>
+      <c r="X7" s="48">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="48"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="1">
+        <v>5</v>
+      </c>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="M9" s="4"/>
+      <c r="O9" s="1">
+        <v>6</v>
+      </c>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="M10" s="4"/>
+      <c r="O10" s="1">
+        <v>7</v>
+      </c>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="M11" s="4"/>
+      <c r="O11" s="1">
+        <v>8</v>
+      </c>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="M12" s="4"/>
+      <c r="O12" s="1">
+        <v>9</v>
+      </c>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48">
+        <v>5</v>
+      </c>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="O16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="O17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="U17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="V17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="X17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y17" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="49">
+        <v>8.94</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="M18" s="4"/>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="49">
+        <v>65</v>
+      </c>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="49"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="M19" s="4"/>
+      <c r="O19" s="1">
+        <v>1</v>
+      </c>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="49"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="M20" s="4"/>
+      <c r="O20" s="1">
+        <v>2</v>
+      </c>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="46"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="M21" s="4"/>
+      <c r="O21" s="1">
+        <v>3</v>
+      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="49"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="49"/>
+      <c r="Y21" s="49"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>4</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="M22" s="4"/>
+      <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="49"/>
+      <c r="V22" s="52"/>
+      <c r="W22" s="52"/>
+      <c r="X22" s="52"/>
+      <c r="Y22" s="52"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>5</v>
+      </c>
+      <c r="B23" s="47"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="M23" s="4"/>
+      <c r="O23" s="1">
+        <v>5</v>
+      </c>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="49"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="52"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>6</v>
+      </c>
+      <c r="B24" s="47"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="M24" s="4"/>
+      <c r="O24" s="1">
+        <v>6</v>
+      </c>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="49"/>
+      <c r="V24" s="52"/>
+      <c r="W24" s="52"/>
+      <c r="X24" s="52"/>
+      <c r="Y24" s="52"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>7</v>
+      </c>
+      <c r="B25" s="47"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="M25" s="4"/>
+      <c r="O25" s="1">
+        <v>7</v>
+      </c>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="49"/>
+      <c r="V25" s="52"/>
+      <c r="W25" s="52"/>
+      <c r="X25" s="52"/>
+      <c r="Y25" s="52"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="24">
+        <v>8</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="M26" s="4"/>
+      <c r="O26" s="1">
+        <v>8</v>
+      </c>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="49"/>
+      <c r="V26" s="52"/>
+      <c r="W26" s="52"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="52"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="24">
+        <v>9</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="M27" s="4"/>
+      <c r="O27" s="1">
+        <v>9</v>
+      </c>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="49"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="49"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="33">
+        <f>AVERAGE(B18:B27)</f>
+        <v>8.94</v>
+      </c>
+      <c r="C28" s="34" t="e">
+        <f>AVERAGE(C18:C27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D28" s="33" t="e">
+        <f>AVERAGE(D18:D27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E28" s="33" t="e">
+        <f>AVERAGE(E18:E27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F28" s="33" t="e">
+        <f>AVERAGE(F18:F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" s="33" t="e">
+        <f>AVERAGE(G18:G27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="33" t="e">
+        <f>AVERAGE(H18:H27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="33" t="e">
+        <f>AVERAGE(I18:I27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" s="33" t="e">
+        <f>AVERAGE(J18:J27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K28" s="33" t="e">
+        <f>AVERAGE(K18:K27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="21">
+        <f>_xlfn.STDEV.P(B18:B27)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="21" t="e">
+        <f>_xlfn.STDEV.P(C18:C27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D29" s="21" t="e">
+        <f>_xlfn.STDEV.P(D18:D27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E29" s="21" t="e">
+        <f>_xlfn.STDEV.P(E18:E27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="21" t="e">
+        <f>_xlfn.STDEV.P(F18:F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="21" t="e">
+        <f>_xlfn.STDEV.P(G18:G27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="21" t="e">
+        <f>_xlfn.STDEV.P(H18:H27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="21" t="e">
+        <f>_xlfn.STDEV.P(I18:I27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="21" t="e">
+        <f>_xlfn.STDEV.P(J18:J27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K29" s="21" t="e">
+        <f>_xlfn.STDEV.P(K18:K27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="18">
+        <v>1</v>
+      </c>
+      <c r="C30" s="19">
+        <v>0</v>
+      </c>
+      <c r="D30" s="19">
+        <v>0</v>
+      </c>
+      <c r="E30" s="19">
+        <v>0</v>
+      </c>
+      <c r="F30" s="19">
+        <v>0</v>
+      </c>
+      <c r="G30" s="19">
+        <v>0</v>
+      </c>
+      <c r="H30" s="19">
+        <v>0</v>
+      </c>
+      <c r="I30" s="19">
+        <v>0</v>
+      </c>
+      <c r="J30" s="20">
+        <v>0</v>
+      </c>
+      <c r="K30" s="32">
+        <v>0</v>
+      </c>
+      <c r="L30" s="32">
+        <f>SUM(B30:K30)</f>
+        <v>1</v>
+      </c>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" s="4"/>
+      <c r="O34" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="P34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" s="4"/>
+      <c r="O35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R35" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="S35" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="T35" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="U35" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="V35" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="X35" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y35" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="M36" s="4"/>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="49"/>
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="49"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
+      <c r="B37" s="46"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="M37" s="4"/>
+      <c r="O37" s="1">
+        <v>1</v>
+      </c>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="49"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="49"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>2</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="M38" s="4"/>
+      <c r="O38" s="1">
+        <v>2</v>
+      </c>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="49"/>
+      <c r="U38" s="49"/>
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49"/>
+      <c r="Y38" s="49"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>3</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="M39" s="4"/>
+      <c r="O39" s="1">
+        <v>3</v>
+      </c>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="49"/>
+      <c r="U39" s="49"/>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="49"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40" s="24">
+        <v>4</v>
+      </c>
+      <c r="B40" s="47"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="M40" s="4"/>
+      <c r="O40" s="1">
+        <v>4</v>
+      </c>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="49"/>
+      <c r="V40" s="52"/>
+      <c r="W40" s="52"/>
+      <c r="X40" s="52"/>
+      <c r="Y40" s="52"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" s="24">
+        <v>5</v>
+      </c>
+      <c r="B41" s="47"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="M41" s="4"/>
+      <c r="O41" s="1">
+        <v>5</v>
+      </c>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="49"/>
+      <c r="V41" s="52"/>
+      <c r="W41" s="52"/>
+      <c r="X41" s="52"/>
+      <c r="Y41" s="52"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" s="24">
+        <v>6</v>
+      </c>
+      <c r="B42" s="47"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="M42" s="4"/>
+      <c r="O42" s="1">
+        <v>6</v>
+      </c>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="52"/>
+      <c r="W42" s="52"/>
+      <c r="X42" s="52"/>
+      <c r="Y42" s="52"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43" s="24">
+        <v>7</v>
+      </c>
+      <c r="B43" s="47"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="M43" s="4"/>
+      <c r="O43" s="1">
+        <v>7</v>
+      </c>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="49"/>
+      <c r="U43" s="49"/>
+      <c r="V43" s="52"/>
+      <c r="W43" s="52"/>
+      <c r="X43" s="52"/>
+      <c r="Y43" s="52"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" s="24">
+        <v>8</v>
+      </c>
+      <c r="B44" s="47"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="M44" s="4"/>
+      <c r="O44" s="1">
+        <v>8</v>
+      </c>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="49"/>
+      <c r="U44" s="49"/>
+      <c r="V44" s="52"/>
+      <c r="W44" s="52"/>
+      <c r="X44" s="52"/>
+      <c r="Y44" s="52"/>
+    </row>
+    <row r="45" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="24">
+        <v>9</v>
+      </c>
+      <c r="B45" s="47"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+      <c r="M45" s="4"/>
+      <c r="O45" s="1">
+        <v>9</v>
+      </c>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="49"/>
+      <c r="S45" s="49"/>
+      <c r="T45" s="49"/>
+      <c r="U45" s="49"/>
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="49"/>
+    </row>
+    <row r="46" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="33" t="e">
+        <f>AVERAGE(B36:B45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C46" s="34" t="e">
+        <f>AVERAGE(C36:C45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" s="33" t="e">
+        <f>AVERAGE(D36:D45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E46" s="33" t="e">
+        <f>AVERAGE(E36:E45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F46" s="33" t="e">
+        <f>AVERAGE(F36:F45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" s="33" t="e">
+        <f>AVERAGE(G36:G45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" s="33" t="e">
+        <f>AVERAGE(H36:H45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" s="33" t="e">
+        <f>AVERAGE(I36:I45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" s="33" t="e">
+        <f>AVERAGE(J36:J45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" s="33" t="e">
+        <f>AVERAGE(K36:K45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="21" t="e">
+        <f>_xlfn.STDEV.P(B36:B45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C47" s="21" t="e">
+        <f>_xlfn.STDEV.P(C36:C45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" s="21" t="e">
+        <f>_xlfn.STDEV.P(D36:D45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" s="21" t="e">
+        <f>_xlfn.STDEV.P(E36:E45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F47" s="21" t="e">
+        <f>_xlfn.STDEV.P(F36:F45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" s="21" t="e">
+        <f>_xlfn.STDEV.P(G36:G45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" s="21" t="e">
+        <f>_xlfn.STDEV.P(H36:H45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" s="21" t="e">
+        <f>_xlfn.STDEV.P(I36:I45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J47" s="21" t="e">
+        <f>_xlfn.STDEV.P(J36:J45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" s="21" t="e">
+        <f>_xlfn.STDEV.P(K36:K45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="18">
+        <v>0</v>
+      </c>
+      <c r="C48" s="19">
+        <v>0</v>
+      </c>
+      <c r="D48" s="19">
+        <v>0</v>
+      </c>
+      <c r="E48" s="19">
+        <v>0</v>
+      </c>
+      <c r="F48" s="19">
+        <v>0</v>
+      </c>
+      <c r="G48" s="19">
+        <v>0</v>
+      </c>
+      <c r="H48" s="19">
+        <v>0</v>
+      </c>
+      <c r="I48" s="19">
+        <v>0</v>
+      </c>
+      <c r="J48" s="20">
+        <v>0</v>
+      </c>
+      <c r="K48" s="32">
+        <f>SUM(B48:J48)</f>
+        <v>0</v>
+      </c>
+      <c r="L48" s="32">
+        <f>SUM(B48:K48)</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="4"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M51" s="4"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>15</v>
+      </c>
+      <c r="M52" s="4"/>
+      <c r="O52" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I53" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K53" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M53" s="4"/>
+      <c r="O53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P53" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R53" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="S53" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="T53" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="U53" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="V53" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W53" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="X53" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y53" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>0</v>
+      </c>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="M54" s="4"/>
+      <c r="O54" s="1">
+        <v>0</v>
+      </c>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="49"/>
+      <c r="U54" s="49"/>
+      <c r="V54" s="49"/>
+      <c r="W54" s="49"/>
+      <c r="X54" s="49"/>
+      <c r="Y54" s="49"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>1</v>
+      </c>
+      <c r="B55" s="50"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="M55" s="4"/>
+      <c r="O55" s="1">
+        <v>1</v>
+      </c>
+      <c r="P55" s="49"/>
+      <c r="Q55" s="49"/>
+      <c r="R55" s="49"/>
+      <c r="S55" s="49"/>
+      <c r="T55" s="49"/>
+      <c r="U55" s="49"/>
+      <c r="V55" s="49"/>
+      <c r="W55" s="49"/>
+      <c r="X55" s="49"/>
+      <c r="Y55" s="49"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>2</v>
+      </c>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="M56" s="4"/>
+      <c r="O56" s="1">
+        <v>2</v>
+      </c>
+      <c r="P56" s="49"/>
+      <c r="Q56" s="49"/>
+      <c r="R56" s="49"/>
+      <c r="S56" s="49"/>
+      <c r="T56" s="49"/>
+      <c r="U56" s="49"/>
+      <c r="V56" s="49"/>
+      <c r="W56" s="49"/>
+      <c r="X56" s="49"/>
+      <c r="Y56" s="49"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>3</v>
+      </c>
+      <c r="B57" s="50"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="49"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="49"/>
+      <c r="M57" s="4"/>
+      <c r="O57" s="1">
+        <v>3</v>
+      </c>
+      <c r="P57" s="49"/>
+      <c r="Q57" s="49"/>
+      <c r="R57" s="49"/>
+      <c r="S57" s="49"/>
+      <c r="T57" s="49"/>
+      <c r="U57" s="49"/>
+      <c r="V57" s="49"/>
+      <c r="W57" s="49"/>
+      <c r="X57" s="49"/>
+      <c r="Y57" s="49"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" s="24">
+        <v>4</v>
+      </c>
+      <c r="B58" s="51"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="52"/>
+      <c r="M58" s="4"/>
+      <c r="O58" s="1">
+        <v>4</v>
+      </c>
+      <c r="P58" s="49"/>
+      <c r="Q58" s="49"/>
+      <c r="R58" s="49"/>
+      <c r="S58" s="49"/>
+      <c r="T58" s="49"/>
+      <c r="U58" s="49"/>
+      <c r="V58" s="52"/>
+      <c r="W58" s="52"/>
+      <c r="X58" s="52"/>
+      <c r="Y58" s="52"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="24">
+        <v>5</v>
+      </c>
+      <c r="B59" s="51"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="M59" s="4"/>
+      <c r="O59" s="1">
+        <v>5</v>
+      </c>
+      <c r="P59" s="49"/>
+      <c r="Q59" s="49"/>
+      <c r="R59" s="49"/>
+      <c r="S59" s="49"/>
+      <c r="T59" s="49"/>
+      <c r="U59" s="49"/>
+      <c r="V59" s="52"/>
+      <c r="W59" s="52"/>
+      <c r="X59" s="52"/>
+      <c r="Y59" s="52"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" s="24">
+        <v>6</v>
+      </c>
+      <c r="B60" s="51"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="52"/>
+      <c r="M60" s="4"/>
+      <c r="O60" s="1">
+        <v>6</v>
+      </c>
+      <c r="P60" s="49"/>
+      <c r="Q60" s="49"/>
+      <c r="R60" s="49"/>
+      <c r="S60" s="49"/>
+      <c r="T60" s="49"/>
+      <c r="U60" s="49"/>
+      <c r="V60" s="52"/>
+      <c r="W60" s="52"/>
+      <c r="X60" s="52"/>
+      <c r="Y60" s="52"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="24">
+        <v>7</v>
+      </c>
+      <c r="B61" s="51"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="52"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="52"/>
+      <c r="M61" s="4"/>
+      <c r="O61" s="1">
+        <v>7</v>
+      </c>
+      <c r="P61" s="49"/>
+      <c r="Q61" s="49"/>
+      <c r="R61" s="49"/>
+      <c r="S61" s="49"/>
+      <c r="T61" s="49"/>
+      <c r="U61" s="49"/>
+      <c r="V61" s="52"/>
+      <c r="W61" s="52"/>
+      <c r="X61" s="52"/>
+      <c r="Y61" s="52"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" s="24">
+        <v>8</v>
+      </c>
+      <c r="B62" s="51"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="52"/>
+      <c r="M62" s="4"/>
+      <c r="O62" s="1">
+        <v>8</v>
+      </c>
+      <c r="P62" s="49"/>
+      <c r="Q62" s="49"/>
+      <c r="R62" s="49"/>
+      <c r="S62" s="49"/>
+      <c r="T62" s="49"/>
+      <c r="U62" s="49"/>
+      <c r="V62" s="52"/>
+      <c r="W62" s="52"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="52"/>
+    </row>
+    <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="24">
+        <v>9</v>
+      </c>
+      <c r="B63" s="51"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="52"/>
+      <c r="M63" s="4"/>
+      <c r="O63" s="1">
+        <v>9</v>
+      </c>
+      <c r="P63" s="49"/>
+      <c r="Q63" s="49"/>
+      <c r="R63" s="49"/>
+      <c r="S63" s="49"/>
+      <c r="T63" s="49"/>
+      <c r="U63" s="49"/>
+      <c r="V63" s="49"/>
+      <c r="W63" s="49"/>
+      <c r="X63" s="49"/>
+      <c r="Y63" s="49"/>
+    </row>
+    <row r="64" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="33" t="e">
+        <f>AVERAGE(B54:B63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C64" s="34" t="e">
+        <f>AVERAGE(C54:C63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D64" s="33" t="e">
+        <f>AVERAGE(D54:D63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E64" s="33" t="e">
+        <f>AVERAGE(E54:E63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F64" s="33" t="e">
+        <f>AVERAGE(F54:F63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G64" s="33" t="e">
+        <f>AVERAGE(G54:G63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H64" s="33" t="e">
+        <f>AVERAGE(H54:H63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" s="33" t="e">
+        <f>AVERAGE(I54:I63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J64" s="33" t="e">
+        <f>AVERAGE(J54:J63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K64" s="33" t="e">
+        <f>AVERAGE(K54:K63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M64" s="4"/>
+    </row>
+    <row r="65" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="21" t="e">
+        <f>_xlfn.STDEV.P(B54:B63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C65" s="21" t="e">
+        <f>_xlfn.STDEV.P(C54:C63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D65" s="21" t="e">
+        <f>_xlfn.STDEV.P(D54:D63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E65" s="21" t="e">
+        <f>_xlfn.STDEV.P(E54:E63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F65" s="21" t="e">
+        <f>_xlfn.STDEV.P(F54:F63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G65" s="21" t="e">
+        <f>_xlfn.STDEV.P(G54:G63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H65" s="21" t="e">
+        <f>_xlfn.STDEV.P(H54:H63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="21" t="e">
+        <f>_xlfn.STDEV.P(I54:I63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J65" s="21" t="e">
+        <f>_xlfn.STDEV.P(J54:J63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K65" s="21" t="e">
+        <f>_xlfn.STDEV.P(K54:K63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M65" s="4"/>
+    </row>
+    <row r="66" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="18">
+        <v>0</v>
+      </c>
+      <c r="C66" s="19">
+        <v>0</v>
+      </c>
+      <c r="D66" s="19">
+        <v>0</v>
+      </c>
+      <c r="E66" s="19">
+        <v>0</v>
+      </c>
+      <c r="F66" s="19">
+        <v>0</v>
+      </c>
+      <c r="G66" s="19">
+        <v>0</v>
+      </c>
+      <c r="H66" s="19">
+        <v>0</v>
+      </c>
+      <c r="I66" s="19">
+        <v>0</v>
+      </c>
+      <c r="J66" s="20">
+        <v>0</v>
+      </c>
+      <c r="K66" s="32">
+        <f>SUM(B66:J66)</f>
+        <v>0</v>
+      </c>
+      <c r="L66" s="32">
+        <f>SUM(B66:K66)</f>
+        <v>0</v>
+      </c>
+      <c r="M66" s="4"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M67" s="4"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="4"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+      <c r="U68" s="4"/>
+      <c r="V68" s="4"/>
+      <c r="W68" s="4"/>
+      <c r="X68" s="4"/>
+      <c r="Y68" s="4"/>
+      <c r="Z68" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing transformTo and ChipsChallenge VGDL
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FD1939-CB3C-4952-93DC-479FAD3CDF5A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFC6A3A-DBD3-4DAC-851E-5EABB3925A00}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +170,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +232,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -369,11 +387,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -484,16 +515,34 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,16 +643,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>21982</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>688732</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>36634</xdr:rowOff>
+      <xdr:rowOff>43961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>293078</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>161192</xdr:rowOff>
+      <xdr:rowOff>168519</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -618,8 +667,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8044963" y="2322634"/>
-          <a:ext cx="1172307" cy="315058"/>
+          <a:off x="7722578" y="2329961"/>
+          <a:ext cx="1194287" cy="315058"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -934,7 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH69"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -3041,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
   <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3085,7 +3134,7 @@
       <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="53" t="s">
+      <c r="X1" s="51" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3162,36 +3211,36 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
       <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="48"/>
       <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
+      <c r="J3" s="56"/>
       <c r="K3" s="48"/>
       <c r="M3" s="4"/>
       <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="52">
         <v>1</v>
       </c>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48">
+      <c r="Q3" s="49"/>
+      <c r="R3" s="52">
         <v>5</v>
       </c>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48">
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="52">
         <v>1</v>
       </c>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="3">
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="9">
         <v>-1</v>
       </c>
     </row>
@@ -3199,34 +3248,34 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="48"/>
       <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="48"/>
       <c r="M4" s="4"/>
       <c r="O4" s="1">
         <v>1</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="3">
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="9">
         <v>-1</v>
       </c>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="48">
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="52">
         <v>1</v>
       </c>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="3">
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="9">
         <v>-1</v>
       </c>
     </row>
@@ -3234,249 +3283,249 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="48"/>
       <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
+      <c r="J5" s="56"/>
       <c r="K5" s="48"/>
       <c r="M5" s="4"/>
       <c r="O5" s="1">
         <v>2</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="3">
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="9">
         <v>-1</v>
       </c>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="48"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="48"/>
       <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
+      <c r="J6" s="56"/>
       <c r="K6" s="48"/>
       <c r="M6" s="4"/>
       <c r="O6" s="1">
         <v>3</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="3">
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="9">
         <v>-1</v>
       </c>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
-      <c r="W6" s="3">
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="9">
         <v>-1</v>
       </c>
-      <c r="X6" s="48">
+      <c r="X6" s="52">
         <v>1</v>
       </c>
-      <c r="Y6" s="48"/>
+      <c r="Y6" s="49"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="48"/>
       <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="48"/>
       <c r="M7" s="4"/>
       <c r="O7" s="1">
         <v>4</v>
       </c>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48">
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="52">
         <v>3</v>
       </c>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48">
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="52">
         <v>1</v>
       </c>
-      <c r="X7" s="48">
+      <c r="X7" s="52">
         <v>1</v>
       </c>
-      <c r="Y7" s="48"/>
+      <c r="Y7" s="49"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="48"/>
       <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
+      <c r="J8" s="56"/>
       <c r="K8" s="48"/>
       <c r="M8" s="4"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="48"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
+      <c r="J9" s="56"/>
       <c r="K9" s="48"/>
       <c r="M9" s="4"/>
       <c r="O9" s="1">
         <v>6</v>
       </c>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
-      <c r="W9" s="48"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="48"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
+      <c r="J10" s="56"/>
       <c r="K10" s="48"/>
       <c r="M10" s="4"/>
       <c r="O10" s="1">
         <v>7</v>
       </c>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="48"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
-      <c r="Y10" s="48"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
+      <c r="J11" s="56"/>
       <c r="K11" s="48"/>
       <c r="M11" s="4"/>
       <c r="O11" s="1">
         <v>8</v>
       </c>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="48"/>
       <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+      <c r="J12" s="56"/>
       <c r="K12" s="48"/>
       <c r="M12" s="4"/>
       <c r="O12" s="1">
         <v>9</v>
       </c>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48">
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="52">
         <v>5</v>
       </c>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="48"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M13" s="4"/>
@@ -3589,7 +3638,7 @@
       <c r="W17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="X17" s="16" t="s">
+      <c r="X17" s="59" t="s">
         <v>8</v>
       </c>
       <c r="Y17" s="16" t="s">
@@ -3600,33 +3649,41 @@
       <c r="A18" s="1">
         <v>0</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="52">
         <v>8.94</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="49"/>
+      <c r="D18" s="54">
+        <v>505.53</v>
+      </c>
       <c r="E18" s="49"/>
       <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
+      <c r="G18" s="56">
+        <v>295.70999999999998</v>
+      </c>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="49"/>
       <c r="M18" s="4"/>
       <c r="O18" s="1">
         <v>0</v>
       </c>
-      <c r="P18" s="49">
+      <c r="P18" s="54">
         <v>65</v>
       </c>
       <c r="Q18" s="9"/>
-      <c r="R18" s="49"/>
+      <c r="R18" s="54">
+        <v>163</v>
+      </c>
       <c r="S18" s="49"/>
       <c r="T18" s="49"/>
-      <c r="U18" s="49"/>
+      <c r="U18" s="57">
+        <v>187</v>
+      </c>
       <c r="V18" s="49"/>
       <c r="W18" s="49"/>
-      <c r="X18" s="49"/>
+      <c r="X18" s="13"/>
       <c r="Y18" s="49"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -3635,13 +3692,15 @@
       </c>
       <c r="B19" s="46"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="49"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
+      <c r="G19" s="56">
+        <v>335.76</v>
+      </c>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="49"/>
       <c r="M19" s="4"/>
       <c r="O19" s="1">
@@ -3649,13 +3708,15 @@
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
-      <c r="R19" s="49"/>
+      <c r="R19" s="9"/>
       <c r="S19" s="49"/>
       <c r="T19" s="49"/>
-      <c r="U19" s="49"/>
+      <c r="U19" s="57">
+        <v>262</v>
+      </c>
       <c r="V19" s="49"/>
       <c r="W19" s="49"/>
-      <c r="X19" s="49"/>
+      <c r="X19" s="13"/>
       <c r="Y19" s="49"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -3664,13 +3725,17 @@
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="49"/>
+      <c r="D20" s="54">
+        <v>258.99</v>
+      </c>
       <c r="E20" s="49"/>
       <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
+      <c r="G20" s="56">
+        <v>885.99</v>
+      </c>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="49"/>
       <c r="M20" s="4"/>
       <c r="O20" s="1">
@@ -3678,13 +3743,17 @@
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
-      <c r="R20" s="49"/>
+      <c r="R20" s="54">
+        <v>136</v>
+      </c>
       <c r="S20" s="49"/>
       <c r="T20" s="49"/>
-      <c r="U20" s="49"/>
+      <c r="U20" s="57">
+        <v>364</v>
+      </c>
       <c r="V20" s="49"/>
       <c r="W20" s="49"/>
-      <c r="X20" s="49"/>
+      <c r="X20" s="13"/>
       <c r="Y20" s="49"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -3693,13 +3762,15 @@
       </c>
       <c r="B21" s="46"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="49"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
+      <c r="J21" s="56">
+        <v>377.76</v>
+      </c>
       <c r="K21" s="49"/>
       <c r="M21" s="4"/>
       <c r="O21" s="1">
@@ -3707,13 +3778,15 @@
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
-      <c r="R21" s="49"/>
+      <c r="R21" s="55"/>
       <c r="S21" s="49"/>
       <c r="T21" s="49"/>
-      <c r="U21" s="49"/>
+      <c r="U21" s="13"/>
       <c r="V21" s="49"/>
       <c r="W21" s="49"/>
-      <c r="X21" s="49"/>
+      <c r="X21" s="57">
+        <v>153</v>
+      </c>
       <c r="Y21" s="49"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -3722,28 +3795,36 @@
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
+      <c r="D22" s="54">
+        <v>158.88</v>
+      </c>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="56">
+        <v>555.86</v>
+      </c>
+      <c r="K22" s="50"/>
       <c r="M22" s="4"/>
       <c r="O22" s="1">
         <v>4</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
-      <c r="R22" s="49"/>
+      <c r="R22" s="54">
+        <v>98</v>
+      </c>
       <c r="S22" s="49"/>
       <c r="T22" s="49"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="52"/>
-      <c r="W22" s="52"/>
-      <c r="X22" s="52"/>
-      <c r="Y22" s="52"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="50"/>
+      <c r="W22" s="50"/>
+      <c r="X22" s="57">
+        <v>133</v>
+      </c>
+      <c r="Y22" s="50"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
@@ -3751,28 +3832,36 @@
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
+      <c r="D23" s="54">
+        <v>385.23</v>
+      </c>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="56">
+        <v>507.3</v>
+      </c>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="50"/>
       <c r="M23" s="4"/>
       <c r="O23" s="1">
         <v>5</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
-      <c r="R23" s="49"/>
+      <c r="R23" s="54">
+        <v>142</v>
+      </c>
       <c r="S23" s="49"/>
       <c r="T23" s="49"/>
-      <c r="U23" s="49"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="52"/>
-      <c r="Y23" s="52"/>
+      <c r="U23" s="57">
+        <v>241</v>
+      </c>
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="50"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
@@ -3780,28 +3869,40 @@
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
+      <c r="D24" s="54">
+        <v>266.64</v>
+      </c>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="56">
+        <v>215.17</v>
+      </c>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="56">
+        <v>124.26</v>
+      </c>
+      <c r="K24" s="50"/>
       <c r="M24" s="4"/>
       <c r="O24" s="1">
         <v>6</v>
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
-      <c r="R24" s="49"/>
+      <c r="R24" s="54">
+        <v>93</v>
+      </c>
       <c r="S24" s="49"/>
       <c r="T24" s="49"/>
-      <c r="U24" s="49"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
-      <c r="Y24" s="52"/>
+      <c r="U24" s="57">
+        <v>154</v>
+      </c>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="57">
+        <v>118</v>
+      </c>
+      <c r="Y24" s="50"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
@@ -3809,28 +3910,40 @@
       </c>
       <c r="B25" s="47"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
+      <c r="D25" s="54">
+        <v>205.66</v>
+      </c>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="56">
+        <v>366.21</v>
+      </c>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="56">
+        <v>710.67</v>
+      </c>
+      <c r="K25" s="50"/>
       <c r="M25" s="4"/>
       <c r="O25" s="1">
         <v>7</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
-      <c r="R25" s="49"/>
+      <c r="R25" s="54">
+        <v>111</v>
+      </c>
       <c r="S25" s="49"/>
       <c r="T25" s="49"/>
-      <c r="U25" s="49"/>
-      <c r="V25" s="52"/>
-      <c r="W25" s="52"/>
-      <c r="X25" s="52"/>
-      <c r="Y25" s="52"/>
+      <c r="U25" s="57">
+        <v>199</v>
+      </c>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="57">
+        <v>148</v>
+      </c>
+      <c r="Y25" s="50"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
@@ -3838,28 +3951,40 @@
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
+      <c r="D26" s="54">
+        <v>63.19</v>
+      </c>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="56">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="56">
+        <v>829.02</v>
+      </c>
+      <c r="K26" s="50"/>
       <c r="M26" s="4"/>
       <c r="O26" s="1">
         <v>8</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
-      <c r="R26" s="49"/>
+      <c r="R26" s="54">
+        <v>106</v>
+      </c>
       <c r="S26" s="49"/>
       <c r="T26" s="49"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="52"/>
-      <c r="X26" s="52"/>
-      <c r="Y26" s="52"/>
+      <c r="U26" s="57">
+        <v>78</v>
+      </c>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="57">
+        <v>258</v>
+      </c>
+      <c r="Y26" s="50"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
@@ -3867,27 +3992,39 @@
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
+      <c r="D27" s="54">
+        <v>252.04</v>
+      </c>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="56">
+        <v>347.65</v>
+      </c>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="56">
+        <v>850.38</v>
+      </c>
+      <c r="K27" s="50"/>
       <c r="M27" s="4"/>
       <c r="O27" s="1">
         <v>9</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
-      <c r="R27" s="49"/>
+      <c r="R27" s="54">
+        <v>169</v>
+      </c>
       <c r="S27" s="49"/>
       <c r="T27" s="49"/>
-      <c r="U27" s="49"/>
+      <c r="U27" s="57">
+        <v>187</v>
+      </c>
       <c r="V27" s="49"/>
       <c r="W27" s="49"/>
-      <c r="X27" s="49"/>
+      <c r="X27" s="57">
+        <v>358</v>
+      </c>
       <c r="Y27" s="49"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3895,43 +4032,43 @@
         <v>18</v>
       </c>
       <c r="B28" s="33">
-        <f>AVERAGE(B18:B27)</f>
+        <f t="shared" ref="B28:K28" si="0">AVERAGE(B18:B27)</f>
         <v>8.94</v>
       </c>
       <c r="C28" s="34" t="e">
-        <f>AVERAGE(C18:C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="33" t="e">
-        <f>AVERAGE(D18:D27)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D28" s="53">
+        <f t="shared" si="0"/>
+        <v>262.02000000000004</v>
       </c>
       <c r="E28" s="33" t="e">
-        <f>AVERAGE(E18:E27)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F28" s="33" t="e">
-        <f>AVERAGE(F18:F27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="33" t="e">
-        <f>AVERAGE(G18:G27)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" s="33">
+        <f t="shared" si="0"/>
+        <v>369.76749999999998</v>
       </c>
       <c r="H28" s="33" t="e">
-        <f>AVERAGE(H18:H27)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I28" s="33" t="e">
-        <f>AVERAGE(I18:I27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J28" s="33" t="e">
-        <f>AVERAGE(J18:J27)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" s="33">
+        <f t="shared" si="0"/>
+        <v>574.65833333333342</v>
       </c>
       <c r="K28" s="33" t="e">
-        <f>AVERAGE(K18:K27)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M28" s="4"/>
@@ -3941,43 +4078,43 @@
         <v>20</v>
       </c>
       <c r="B29" s="21">
-        <f>_xlfn.STDEV.P(B18:B27)</f>
+        <f t="shared" ref="B29:K29" si="1">_xlfn.STDEV.P(B18:B27)</f>
         <v>0</v>
       </c>
       <c r="C29" s="21" t="e">
-        <f>_xlfn.STDEV.P(C18:C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D29" s="21" t="e">
-        <f>_xlfn.STDEV.P(D18:D27)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D29" s="21">
+        <f t="shared" si="1"/>
+        <v>126.46918004003969</v>
       </c>
       <c r="E29" s="21" t="e">
-        <f>_xlfn.STDEV.P(E18:E27)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F29" s="21" t="e">
-        <f>_xlfn.STDEV.P(F18:F27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="21" t="e">
-        <f>_xlfn.STDEV.P(G18:G27)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="21">
+        <f t="shared" si="1"/>
+        <v>237.16398792554915</v>
       </c>
       <c r="H29" s="21" t="e">
-        <f>_xlfn.STDEV.P(H18:H27)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I29" s="21" t="e">
-        <f>_xlfn.STDEV.P(I18:I27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J29" s="21" t="e">
-        <f>_xlfn.STDEV.P(J18:J27)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="21">
+        <f t="shared" si="1"/>
+        <v>258.58669019735362</v>
       </c>
       <c r="K29" s="21" t="e">
-        <f>_xlfn.STDEV.P(K18:K27)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M29" s="4"/>
@@ -3993,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E30" s="19">
         <v>0</v>
@@ -4002,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H30" s="19">
         <v>0</v>
@@ -4011,14 +4148,14 @@
         <v>0</v>
       </c>
       <c r="J30" s="20">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K30" s="32">
         <v>0</v>
       </c>
       <c r="L30" s="32">
         <f>SUM(B30:K30)</f>
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M30" s="4"/>
     </row>
@@ -4146,13 +4283,19 @@
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="49"/>
+      <c r="D36" s="56">
+        <v>4.5584199999999999</v>
+      </c>
       <c r="E36" s="49"/>
       <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
+      <c r="G36" s="56">
+        <v>0.12731100000000001</v>
+      </c>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
+      <c r="J36" s="56">
+        <v>0.11088199999999999</v>
+      </c>
       <c r="K36" s="49"/>
       <c r="M36" s="4"/>
       <c r="O36" s="1">
@@ -4160,13 +4303,19 @@
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
-      <c r="R36" s="49"/>
+      <c r="R36" s="54">
+        <v>142</v>
+      </c>
       <c r="S36" s="49"/>
       <c r="T36" s="49"/>
-      <c r="U36" s="49"/>
+      <c r="U36" s="57">
+        <v>187</v>
+      </c>
       <c r="V36" s="49"/>
       <c r="W36" s="49"/>
-      <c r="X36" s="49"/>
+      <c r="X36" s="57">
+        <v>153</v>
+      </c>
       <c r="Y36" s="49"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -4175,13 +4324,19 @@
       </c>
       <c r="B37" s="46"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="49"/>
+      <c r="D37" s="56">
+        <v>369.37900000000002</v>
+      </c>
       <c r="E37" s="49"/>
       <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
+      <c r="G37" s="56">
+        <v>0.137241</v>
+      </c>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
+      <c r="J37" s="56">
+        <v>0.114484</v>
+      </c>
       <c r="K37" s="49"/>
       <c r="M37" s="4"/>
       <c r="O37" s="1">
@@ -4189,13 +4344,19 @@
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
-      <c r="R37" s="49"/>
+      <c r="R37" s="54">
+        <v>175</v>
+      </c>
       <c r="S37" s="49"/>
       <c r="T37" s="49"/>
-      <c r="U37" s="49"/>
+      <c r="U37" s="57">
+        <v>238</v>
+      </c>
       <c r="V37" s="49"/>
       <c r="W37" s="49"/>
-      <c r="X37" s="49"/>
+      <c r="X37" s="57">
+        <v>208</v>
+      </c>
       <c r="Y37" s="49"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
@@ -4204,13 +4365,19 @@
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="49"/>
+      <c r="D38" s="56">
+        <v>244.98400000000001</v>
+      </c>
       <c r="E38" s="49"/>
       <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
+      <c r="G38" s="56">
+        <v>0.145514</v>
+      </c>
       <c r="H38" s="49"/>
       <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
+      <c r="J38" s="56">
+        <v>0.115649</v>
+      </c>
       <c r="K38" s="49"/>
       <c r="M38" s="4"/>
       <c r="O38" s="1">
@@ -4218,13 +4385,19 @@
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
-      <c r="R38" s="49"/>
+      <c r="R38" s="54">
+        <v>130</v>
+      </c>
       <c r="S38" s="49"/>
       <c r="T38" s="49"/>
-      <c r="U38" s="49"/>
+      <c r="U38" s="57">
+        <v>256</v>
+      </c>
       <c r="V38" s="49"/>
       <c r="W38" s="49"/>
-      <c r="X38" s="49"/>
+      <c r="X38" s="57">
+        <v>208</v>
+      </c>
       <c r="Y38" s="49"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -4233,13 +4406,19 @@
       </c>
       <c r="B39" s="46"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="49"/>
+      <c r="D39" s="56">
+        <v>88.552000000000007</v>
+      </c>
       <c r="E39" s="49"/>
       <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
+      <c r="G39" s="56">
+        <v>0.13156599999999999</v>
+      </c>
       <c r="H39" s="49"/>
       <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
+      <c r="J39" s="56">
+        <v>8.8751200000000002E-2</v>
+      </c>
       <c r="K39" s="49"/>
       <c r="M39" s="4"/>
       <c r="O39" s="1">
@@ -4247,13 +4426,19 @@
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="9"/>
-      <c r="R39" s="49"/>
+      <c r="R39" s="54">
+        <v>134</v>
+      </c>
       <c r="S39" s="49"/>
       <c r="T39" s="49"/>
-      <c r="U39" s="49"/>
+      <c r="U39" s="57">
+        <v>208</v>
+      </c>
       <c r="V39" s="49"/>
       <c r="W39" s="49"/>
-      <c r="X39" s="49"/>
+      <c r="X39" s="57">
+        <v>148</v>
+      </c>
       <c r="Y39" s="49"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
@@ -4262,28 +4447,40 @@
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="10"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
+      <c r="D40" s="56">
+        <v>3.7271200000000002</v>
+      </c>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="56">
+        <v>0.16553699999999999</v>
+      </c>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="56">
+        <v>8.2298700000000002E-2</v>
+      </c>
+      <c r="K40" s="50"/>
       <c r="M40" s="4"/>
       <c r="O40" s="1">
         <v>4</v>
       </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="9"/>
-      <c r="R40" s="49"/>
+      <c r="R40" s="54">
+        <v>89</v>
+      </c>
       <c r="S40" s="49"/>
       <c r="T40" s="49"/>
-      <c r="U40" s="49"/>
-      <c r="V40" s="52"/>
-      <c r="W40" s="52"/>
-      <c r="X40" s="52"/>
-      <c r="Y40" s="52"/>
+      <c r="U40" s="57">
+        <v>379</v>
+      </c>
+      <c r="V40" s="50"/>
+      <c r="W40" s="50"/>
+      <c r="X40" s="57">
+        <v>118</v>
+      </c>
+      <c r="Y40" s="50"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
@@ -4291,28 +4488,40 @@
       </c>
       <c r="B41" s="47"/>
       <c r="C41" s="10"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
+      <c r="D41" s="56">
+        <v>0.64394700000000005</v>
+      </c>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="56">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="56">
+        <v>0.11194</v>
+      </c>
+      <c r="K41" s="50"/>
       <c r="M41" s="4"/>
       <c r="O41" s="1">
         <v>5</v>
       </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
-      <c r="R41" s="49"/>
+      <c r="R41" s="54">
+        <v>103</v>
+      </c>
       <c r="S41" s="49"/>
       <c r="T41" s="49"/>
-      <c r="U41" s="49"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="52"/>
+      <c r="U41" s="57">
+        <v>199</v>
+      </c>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="57">
+        <v>148</v>
+      </c>
+      <c r="Y41" s="50"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="24">
@@ -4320,28 +4529,40 @@
       </c>
       <c r="B42" s="47"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
+      <c r="D42" s="56">
+        <v>0.41857299999999997</v>
+      </c>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="56">
+        <v>0.108722</v>
+      </c>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="56">
+        <v>9.5584500000000003E-2</v>
+      </c>
+      <c r="K42" s="50"/>
       <c r="M42" s="4"/>
       <c r="O42" s="1">
         <v>6</v>
       </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
-      <c r="R42" s="49"/>
+      <c r="R42" s="54">
+        <v>93</v>
+      </c>
       <c r="S42" s="49"/>
       <c r="T42" s="49"/>
-      <c r="U42" s="49"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="52"/>
-      <c r="X42" s="52"/>
-      <c r="Y42" s="52"/>
+      <c r="U42" s="57">
+        <v>154</v>
+      </c>
+      <c r="V42" s="50"/>
+      <c r="W42" s="50"/>
+      <c r="X42" s="57">
+        <v>98</v>
+      </c>
+      <c r="Y42" s="50"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="24">
@@ -4349,28 +4570,40 @@
       </c>
       <c r="B43" s="47"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="52"/>
+      <c r="D43" s="56">
+        <v>0.33063700000000001</v>
+      </c>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="56">
+        <v>0.106403</v>
+      </c>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="56">
+        <v>0.10772</v>
+      </c>
+      <c r="K43" s="50"/>
       <c r="M43" s="4"/>
       <c r="O43" s="1">
         <v>7</v>
       </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="9"/>
-      <c r="R43" s="49"/>
+      <c r="R43" s="54">
+        <v>99</v>
+      </c>
       <c r="S43" s="49"/>
       <c r="T43" s="49"/>
-      <c r="U43" s="49"/>
-      <c r="V43" s="52"/>
-      <c r="W43" s="52"/>
-      <c r="X43" s="52"/>
-      <c r="Y43" s="52"/>
+      <c r="U43" s="57">
+        <v>199</v>
+      </c>
+      <c r="V43" s="50"/>
+      <c r="W43" s="50"/>
+      <c r="X43" s="57">
+        <v>138</v>
+      </c>
+      <c r="Y43" s="50"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="24">
@@ -4378,28 +4611,40 @@
       </c>
       <c r="B44" s="47"/>
       <c r="C44" s="10"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
+      <c r="D44" s="56">
+        <v>0.33985700000000002</v>
+      </c>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="56">
+        <v>7.9479599999999997E-2</v>
+      </c>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="56">
+        <v>0.11412799999999999</v>
+      </c>
+      <c r="K44" s="50"/>
       <c r="M44" s="4"/>
       <c r="O44" s="1">
         <v>8</v>
       </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
-      <c r="R44" s="49"/>
+      <c r="R44" s="54">
+        <v>106</v>
+      </c>
       <c r="S44" s="49"/>
       <c r="T44" s="49"/>
-      <c r="U44" s="49"/>
-      <c r="V44" s="52"/>
-      <c r="W44" s="52"/>
-      <c r="X44" s="52"/>
-      <c r="Y44" s="52"/>
+      <c r="U44" s="57">
+        <v>72</v>
+      </c>
+      <c r="V44" s="50"/>
+      <c r="W44" s="50"/>
+      <c r="X44" s="57">
+        <v>258</v>
+      </c>
+      <c r="Y44" s="50"/>
     </row>
     <row r="45" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24">
@@ -4407,27 +4652,39 @@
       </c>
       <c r="B45" s="47"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="52"/>
+      <c r="D45" s="56">
+        <v>0.54566099999999995</v>
+      </c>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="56">
+        <v>7.1677299999999999E-2</v>
+      </c>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="56">
+        <v>0.15307000000000001</v>
+      </c>
+      <c r="K45" s="50"/>
       <c r="M45" s="4"/>
       <c r="O45" s="1">
         <v>9</v>
       </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="9"/>
-      <c r="R45" s="49"/>
+      <c r="R45" s="54">
+        <v>136</v>
+      </c>
       <c r="S45" s="49"/>
       <c r="T45" s="49"/>
-      <c r="U45" s="49"/>
+      <c r="U45" s="57">
+        <v>187</v>
+      </c>
       <c r="V45" s="49"/>
       <c r="W45" s="49"/>
-      <c r="X45" s="49"/>
+      <c r="X45" s="57">
+        <v>358</v>
+      </c>
       <c r="Y45" s="49"/>
     </row>
     <row r="46" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4435,43 +4692,43 @@
         <v>18</v>
       </c>
       <c r="B46" s="33" t="e">
-        <f>AVERAGE(B36:B45)</f>
+        <f t="shared" ref="B46:K46" si="2">AVERAGE(B36:B45)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C46" s="34" t="e">
-        <f>AVERAGE(C36:C45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D46" s="33" t="e">
-        <f>AVERAGE(D36:D45)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" s="33">
+        <f t="shared" si="2"/>
+        <v>71.347921500000012</v>
       </c>
       <c r="E46" s="33" t="e">
-        <f>AVERAGE(E36:E45)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F46" s="33" t="e">
-        <f>AVERAGE(F36:F45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G46" s="33" t="e">
-        <f>AVERAGE(G36:G45)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" s="33">
+        <f t="shared" si="2"/>
+        <v>0.11856508999999997</v>
       </c>
       <c r="H46" s="33" t="e">
-        <f>AVERAGE(H36:H45)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" s="33" t="e">
-        <f>AVERAGE(I36:I45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J46" s="33" t="e">
-        <f>AVERAGE(J36:J45)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" s="33">
+        <f t="shared" si="2"/>
+        <v>0.10945073999999999</v>
       </c>
       <c r="K46" s="33" t="e">
-        <f>AVERAGE(K36:K45)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M46" s="4"/>
@@ -4481,43 +4738,43 @@
         <v>20</v>
       </c>
       <c r="B47" s="21" t="e">
-        <f>_xlfn.STDEV.P(B36:B45)</f>
+        <f t="shared" ref="B47:K47" si="3">_xlfn.STDEV.P(B36:B45)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C47" s="21" t="e">
-        <f>_xlfn.STDEV.P(C36:C45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D47" s="21" t="e">
-        <f>_xlfn.STDEV.P(D36:D45)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" s="21">
+        <f t="shared" si="3"/>
+        <v>123.86685861614376</v>
       </c>
       <c r="E47" s="21" t="e">
-        <f>_xlfn.STDEV.P(E36:E45)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F47" s="21" t="e">
-        <f>_xlfn.STDEV.P(F36:F45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G47" s="21" t="e">
-        <f>_xlfn.STDEV.P(G36:G45)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" s="21">
+        <f t="shared" si="3"/>
+        <v>2.7456084754329136E-2</v>
       </c>
       <c r="H47" s="21" t="e">
-        <f>_xlfn.STDEV.P(H36:H45)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" s="21" t="e">
-        <f>_xlfn.STDEV.P(I36:I45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J47" s="21" t="e">
-        <f>_xlfn.STDEV.P(J36:J45)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J47" s="21">
+        <f t="shared" si="3"/>
+        <v>1.8323443898197844E-2</v>
       </c>
       <c r="K47" s="21" t="e">
-        <f>_xlfn.STDEV.P(K36:K45)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M47" s="4"/>
@@ -4533,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E48" s="19">
         <v>0</v>
@@ -4542,7 +4799,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H48" s="19">
         <v>0</v>
@@ -4551,15 +4808,14 @@
         <v>0</v>
       </c>
       <c r="J48" s="20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K48" s="32">
-        <f>SUM(B48:J48)</f>
         <v>0</v>
       </c>
       <c r="L48" s="32">
         <f>SUM(B48:K48)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M48" s="4"/>
     </row>
@@ -4685,22 +4941,38 @@
       <c r="A54" s="1">
         <v>0</v>
       </c>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
+      <c r="B54" s="56">
+        <v>1.12389E-2</v>
+      </c>
+      <c r="C54" s="56">
+        <v>42.491300000000003</v>
+      </c>
+      <c r="D54" s="56">
+        <v>6.0726300000000002</v>
+      </c>
+      <c r="E54" s="56">
+        <v>18.004999999999999</v>
+      </c>
       <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
+      <c r="G54" s="56">
+        <v>0.47940199999999999</v>
+      </c>
       <c r="H54" s="49"/>
       <c r="I54" s="49"/>
-      <c r="J54" s="49"/>
+      <c r="J54" s="49">
+        <v>2.0734300000000001</v>
+      </c>
       <c r="K54" s="49"/>
       <c r="M54" s="4"/>
       <c r="O54" s="1">
         <v>0</v>
       </c>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="49"/>
+      <c r="P54" s="57">
+        <v>21</v>
+      </c>
+      <c r="Q54" s="57">
+        <v>258</v>
+      </c>
       <c r="R54" s="49"/>
       <c r="S54" s="49"/>
       <c r="T54" s="49"/>
@@ -4714,12 +4986,22 @@
       <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="49"/>
+      <c r="B55" s="56">
+        <v>6.6536600000000004</v>
+      </c>
+      <c r="C55" s="56">
+        <v>30.741700000000002</v>
+      </c>
+      <c r="D55" s="56">
+        <v>10.238099999999999</v>
+      </c>
+      <c r="E55" s="56">
+        <v>44.814300000000003</v>
+      </c>
       <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
+      <c r="G55" s="56">
+        <v>0.38312600000000002</v>
+      </c>
       <c r="H55" s="49"/>
       <c r="I55" s="49"/>
       <c r="J55" s="49"/>
@@ -4728,8 +5010,12 @@
       <c r="O55" s="1">
         <v>1</v>
       </c>
-      <c r="P55" s="49"/>
-      <c r="Q55" s="49"/>
+      <c r="P55" s="57">
+        <v>121</v>
+      </c>
+      <c r="Q55" s="57">
+        <v>208</v>
+      </c>
       <c r="R55" s="49"/>
       <c r="S55" s="49"/>
       <c r="T55" s="49"/>
@@ -4743,12 +5029,22 @@
       <c r="A56" s="1">
         <v>2</v>
       </c>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
+      <c r="B56" s="56">
+        <v>0.16361800000000001</v>
+      </c>
+      <c r="C56" s="56">
+        <v>25.808399999999999</v>
+      </c>
+      <c r="D56" s="56">
+        <v>8.8827600000000007E-2</v>
+      </c>
+      <c r="E56" s="56">
+        <v>19.5749</v>
+      </c>
       <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
+      <c r="G56" s="56">
+        <v>0.50300400000000001</v>
+      </c>
       <c r="H56" s="49"/>
       <c r="I56" s="49"/>
       <c r="J56" s="49"/>
@@ -4757,8 +5053,12 @@
       <c r="O56" s="1">
         <v>2</v>
       </c>
-      <c r="P56" s="49"/>
-      <c r="Q56" s="49"/>
+      <c r="P56" s="57">
+        <v>42</v>
+      </c>
+      <c r="Q56" s="57">
+        <v>175</v>
+      </c>
       <c r="R56" s="49"/>
       <c r="S56" s="49"/>
       <c r="T56" s="49"/>
@@ -4772,12 +5072,22 @@
       <c r="A57" s="1">
         <v>3</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
+      <c r="B57" s="56">
+        <v>17.5992</v>
+      </c>
+      <c r="C57" s="56">
+        <v>49.455800000000004</v>
+      </c>
+      <c r="D57" s="56">
+        <v>9.7938299999999998</v>
+      </c>
+      <c r="E57" s="56">
+        <v>18.940899999999999</v>
+      </c>
       <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
+      <c r="G57" s="56">
+        <v>0.54791000000000001</v>
+      </c>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
       <c r="J57" s="49"/>
@@ -4786,8 +5096,12 @@
       <c r="O57" s="1">
         <v>3</v>
       </c>
-      <c r="P57" s="49"/>
-      <c r="Q57" s="49"/>
+      <c r="P57" s="57">
+        <v>82</v>
+      </c>
+      <c r="Q57" s="57">
+        <v>349</v>
+      </c>
       <c r="R57" s="49"/>
       <c r="S57" s="49"/>
       <c r="T57" s="49"/>
@@ -4801,167 +5115,251 @@
       <c r="A58" s="24">
         <v>4</v>
       </c>
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="52"/>
+      <c r="B58" s="56">
+        <v>29.069099999999999</v>
+      </c>
+      <c r="C58" s="56">
+        <v>2.6156700000000002</v>
+      </c>
+      <c r="D58" s="56">
+        <v>6.22377</v>
+      </c>
+      <c r="E58" s="56">
+        <v>13.1508</v>
+      </c>
+      <c r="F58" s="50"/>
+      <c r="G58" s="56">
+        <v>0.70573300000000005</v>
+      </c>
+      <c r="H58" s="50"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="50"/>
+      <c r="K58" s="50"/>
       <c r="M58" s="4"/>
       <c r="O58" s="1">
         <v>4</v>
       </c>
-      <c r="P58" s="49"/>
-      <c r="Q58" s="49"/>
+      <c r="P58" s="57">
+        <v>137</v>
+      </c>
+      <c r="Q58" s="57">
+        <v>102</v>
+      </c>
       <c r="R58" s="49"/>
       <c r="S58" s="49"/>
       <c r="T58" s="49"/>
       <c r="U58" s="49"/>
-      <c r="V58" s="52"/>
-      <c r="W58" s="52"/>
-      <c r="X58" s="52"/>
-      <c r="Y58" s="52"/>
+      <c r="V58" s="50"/>
+      <c r="W58" s="50"/>
+      <c r="X58" s="50"/>
+      <c r="Y58" s="50"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="24">
         <v>5</v>
       </c>
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="52"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="52"/>
-      <c r="J59" s="52"/>
-      <c r="K59" s="52"/>
+      <c r="B59" s="56">
+        <v>0.132461</v>
+      </c>
+      <c r="C59" s="56">
+        <v>15.929600000000001</v>
+      </c>
+      <c r="D59" s="56">
+        <v>4.43478E-2</v>
+      </c>
+      <c r="E59" s="56">
+        <v>35.987299999999998</v>
+      </c>
+      <c r="F59" s="50"/>
+      <c r="G59" s="56">
+        <v>0.43384499999999998</v>
+      </c>
+      <c r="H59" s="50"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="50"/>
+      <c r="K59" s="50"/>
       <c r="M59" s="4"/>
       <c r="O59" s="1">
         <v>5</v>
       </c>
-      <c r="P59" s="49"/>
-      <c r="Q59" s="49"/>
+      <c r="P59" s="57">
+        <v>77</v>
+      </c>
+      <c r="Q59" s="57">
+        <v>163</v>
+      </c>
       <c r="R59" s="49"/>
       <c r="S59" s="49"/>
       <c r="T59" s="49"/>
       <c r="U59" s="49"/>
-      <c r="V59" s="52"/>
-      <c r="W59" s="52"/>
-      <c r="X59" s="52"/>
-      <c r="Y59" s="52"/>
+      <c r="V59" s="50"/>
+      <c r="W59" s="50"/>
+      <c r="X59" s="50"/>
+      <c r="Y59" s="50"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="24">
         <v>6</v>
       </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="52"/>
-      <c r="H60" s="52"/>
-      <c r="I60" s="52"/>
-      <c r="J60" s="52"/>
-      <c r="K60" s="52"/>
+      <c r="B60" s="56">
+        <v>40.249200000000002</v>
+      </c>
+      <c r="C60" s="56">
+        <v>23.0289</v>
+      </c>
+      <c r="D60" s="56">
+        <v>4.2488100000000001E-2</v>
+      </c>
+      <c r="E60" s="56">
+        <v>21.556999999999999</v>
+      </c>
+      <c r="F60" s="50"/>
+      <c r="G60" s="56">
+        <v>0.44375300000000001</v>
+      </c>
+      <c r="H60" s="50"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="50"/>
       <c r="M60" s="4"/>
       <c r="O60" s="1">
         <v>6</v>
       </c>
-      <c r="P60" s="49"/>
-      <c r="Q60" s="49"/>
+      <c r="P60" s="57">
+        <v>327</v>
+      </c>
+      <c r="Q60" s="57">
+        <v>203</v>
+      </c>
       <c r="R60" s="49"/>
       <c r="S60" s="49"/>
       <c r="T60" s="49"/>
       <c r="U60" s="49"/>
-      <c r="V60" s="52"/>
-      <c r="W60" s="52"/>
-      <c r="X60" s="52"/>
-      <c r="Y60" s="52"/>
+      <c r="V60" s="50"/>
+      <c r="W60" s="50"/>
+      <c r="X60" s="50"/>
+      <c r="Y60" s="50"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="24">
         <v>7</v>
       </c>
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="52"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="52"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="52"/>
+      <c r="B61" s="56">
+        <v>512.66999999999996</v>
+      </c>
+      <c r="C61" s="56">
+        <v>11.9932</v>
+      </c>
+      <c r="D61" s="56">
+        <v>4.3576899999999998</v>
+      </c>
+      <c r="E61" s="56">
+        <v>24.514700000000001</v>
+      </c>
+      <c r="F61" s="50"/>
+      <c r="G61" s="56">
+        <v>0.37591000000000002</v>
+      </c>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
       <c r="M61" s="4"/>
       <c r="O61" s="1">
         <v>7</v>
       </c>
-      <c r="P61" s="49"/>
-      <c r="Q61" s="49"/>
+      <c r="P61" s="57">
+        <v>336</v>
+      </c>
+      <c r="Q61" s="57">
+        <v>227</v>
+      </c>
       <c r="R61" s="49"/>
       <c r="S61" s="49"/>
       <c r="T61" s="49"/>
       <c r="U61" s="49"/>
-      <c r="V61" s="52"/>
-      <c r="W61" s="52"/>
-      <c r="X61" s="52"/>
-      <c r="Y61" s="52"/>
+      <c r="V61" s="50"/>
+      <c r="W61" s="50"/>
+      <c r="X61" s="50"/>
+      <c r="Y61" s="50"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>8</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="52"/>
+      <c r="B62" s="56">
+        <v>20.802</v>
+      </c>
+      <c r="C62" s="56">
+        <v>12.725</v>
+      </c>
+      <c r="D62" s="56">
+        <v>3.2014999999999998</v>
+      </c>
+      <c r="E62" s="56">
+        <v>11.315799999999999</v>
+      </c>
+      <c r="F62" s="50"/>
+      <c r="G62" s="56">
+        <v>0.30377300000000002</v>
+      </c>
+      <c r="H62" s="50"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="50"/>
+      <c r="K62" s="50"/>
       <c r="M62" s="4"/>
       <c r="O62" s="1">
         <v>8</v>
       </c>
-      <c r="P62" s="49"/>
-      <c r="Q62" s="49"/>
+      <c r="P62" s="57">
+        <v>227</v>
+      </c>
+      <c r="Q62" s="57">
+        <v>254</v>
+      </c>
       <c r="R62" s="49"/>
       <c r="S62" s="49"/>
       <c r="T62" s="49"/>
       <c r="U62" s="49"/>
-      <c r="V62" s="52"/>
-      <c r="W62" s="52"/>
-      <c r="X62" s="52"/>
-      <c r="Y62" s="52"/>
+      <c r="V62" s="50"/>
+      <c r="W62" s="50"/>
+      <c r="X62" s="50"/>
+      <c r="Y62" s="50"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="24">
         <v>9</v>
       </c>
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="52"/>
-      <c r="J63" s="52"/>
-      <c r="K63" s="52"/>
+      <c r="B63" s="56">
+        <v>565.20100000000002</v>
+      </c>
+      <c r="C63" s="56">
+        <v>14.2669</v>
+      </c>
+      <c r="D63" s="56">
+        <v>4.6919500000000003</v>
+      </c>
+      <c r="E63" s="56">
+        <v>12.3293</v>
+      </c>
+      <c r="F63" s="50"/>
+      <c r="G63" s="56">
+        <v>0.38303500000000001</v>
+      </c>
+      <c r="H63" s="50"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="50"/>
       <c r="M63" s="4"/>
       <c r="O63" s="1">
         <v>9</v>
       </c>
-      <c r="P63" s="49"/>
-      <c r="Q63" s="49"/>
+      <c r="P63" s="57">
+        <v>313</v>
+      </c>
+      <c r="Q63" s="57">
+        <v>175</v>
+      </c>
       <c r="R63" s="49"/>
       <c r="S63" s="49"/>
       <c r="T63" s="49"/>
@@ -4975,44 +5373,44 @@
       <c r="A64" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="33" t="e">
-        <f>AVERAGE(B54:B63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C64" s="34" t="e">
-        <f>AVERAGE(C54:C63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D64" s="33" t="e">
-        <f>AVERAGE(D54:D63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E64" s="33" t="e">
-        <f>AVERAGE(E54:E63)</f>
-        <v>#DIV/0!</v>
+      <c r="B64" s="33">
+        <f t="shared" ref="B64:K64" si="4">AVERAGE(B54:B63)</f>
+        <v>119.25514779</v>
+      </c>
+      <c r="C64" s="34">
+        <f t="shared" si="4"/>
+        <v>22.905646999999998</v>
+      </c>
+      <c r="D64" s="33">
+        <f t="shared" si="4"/>
+        <v>4.4755133499999991</v>
+      </c>
+      <c r="E64" s="33">
+        <f t="shared" si="4"/>
+        <v>22.018999999999998</v>
       </c>
       <c r="F64" s="33" t="e">
-        <f>AVERAGE(F54:F63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G64" s="33" t="e">
-        <f>AVERAGE(G54:G63)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G64" s="33">
+        <f t="shared" si="4"/>
+        <v>0.45594909999999994</v>
       </c>
       <c r="H64" s="33" t="e">
-        <f>AVERAGE(H54:H63)</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I64" s="33" t="e">
-        <f>AVERAGE(I54:I63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J64" s="33" t="e">
-        <f>AVERAGE(J54:J63)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J64" s="33">
+        <f t="shared" si="4"/>
+        <v>2.0734300000000001</v>
       </c>
       <c r="K64" s="33" t="e">
-        <f>AVERAGE(K54:K63)</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M64" s="4"/>
@@ -5021,44 +5419,44 @@
       <c r="A65" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="21" t="e">
-        <f>_xlfn.STDEV.P(B54:B63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C65" s="21" t="e">
-        <f>_xlfn.STDEV.P(C54:C63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D65" s="21" t="e">
-        <f>_xlfn.STDEV.P(D54:D63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E65" s="21" t="e">
-        <f>_xlfn.STDEV.P(E54:E63)</f>
-        <v>#DIV/0!</v>
+      <c r="B65" s="21">
+        <f t="shared" ref="B65:K65" si="5">_xlfn.STDEV.P(B54:B63)</f>
+        <v>210.55084371985251</v>
+      </c>
+      <c r="C65" s="21">
+        <f t="shared" si="5"/>
+        <v>13.842170139334407</v>
+      </c>
+      <c r="D65" s="21">
+        <f t="shared" si="5"/>
+        <v>3.5680929058188222</v>
+      </c>
+      <c r="E65" s="21">
+        <f t="shared" si="5"/>
+        <v>10.197231670703582</v>
       </c>
       <c r="F65" s="21" t="e">
-        <f>_xlfn.STDEV.P(F54:F63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G65" s="21" t="e">
-        <f>_xlfn.STDEV.P(G54:G63)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G65" s="21">
+        <f t="shared" si="5"/>
+        <v>0.10697375139018937</v>
       </c>
       <c r="H65" s="21" t="e">
-        <f>_xlfn.STDEV.P(H54:H63)</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I65" s="21" t="e">
-        <f>_xlfn.STDEV.P(I54:I63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J65" s="21" t="e">
-        <f>_xlfn.STDEV.P(J54:J63)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J65" s="21">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="K65" s="21" t="e">
-        <f>_xlfn.STDEV.P(K54:K63)</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M65" s="4"/>
@@ -5068,22 +5466,22 @@
         <v>13</v>
       </c>
       <c r="B66" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C66" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D66" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E66" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F66" s="19">
         <v>0</v>
       </c>
       <c r="G66" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H66" s="19">
         <v>0</v>
@@ -5095,12 +5493,11 @@
         <v>0</v>
       </c>
       <c r="K66" s="32">
-        <f>SUM(B66:J66)</f>
         <v>0</v>
       </c>
       <c r="L66" s="32">
         <f>SUM(B66:K66)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M66" s="4"/>
     </row>

</xml_diff>

<commit_message>
Modifying zenpuzzle VGDL. Changing exception message when plan parser fails
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4833B38-E151-4647-AABB-AB5E567C7096}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A7F7CF-D072-4CA1-9C51-6363A2EFF550}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="41">
   <si>
     <t>GVGAI level</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Agent victories only</t>
+  </si>
+  <si>
+    <t>FD (A*)</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -511,7 +514,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,6 +543,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -644,15 +657,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>688732</xdr:colOff>
+      <xdr:colOff>102578</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>43961</xdr:rowOff>
+      <xdr:rowOff>73268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>168519</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>7326</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -667,8 +680,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7722578" y="2329961"/>
-          <a:ext cx="1194287" cy="315058"/>
+          <a:off x="7136424" y="2359268"/>
+          <a:ext cx="1970941" cy="315058"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,7 +721,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> 15 min</a:t>
+            <a:t> 15 min || RAM &gt; 6GB</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -983,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH69"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -3090,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
   <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3134,7 +3147,7 @@
       <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="X1" s="50" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3211,35 +3224,35 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="48"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="59"/>
       <c r="M3" s="4"/>
       <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="P3" s="52">
+      <c r="P3" s="51">
         <v>1</v>
       </c>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="52">
+      <c r="Q3" s="48"/>
+      <c r="R3" s="51">
         <v>5</v>
       </c>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="52">
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="51">
         <v>1</v>
       </c>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
       <c r="Y3" s="9">
         <v>-1</v>
       </c>
@@ -3248,33 +3261,33 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="48"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="59"/>
       <c r="M4" s="4"/>
       <c r="O4" s="1">
         <v>1</v>
       </c>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
       <c r="R4" s="9">
         <v>-1</v>
       </c>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="52">
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="51">
         <v>1</v>
       </c>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
       <c r="Y4" s="9">
         <v>-1</v>
       </c>
@@ -3283,249 +3296,251 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="48"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="59"/>
       <c r="M5" s="4"/>
       <c r="O5" s="1">
         <v>2</v>
       </c>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
       <c r="R5" s="9">
         <v>-1</v>
       </c>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="48"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="59"/>
       <c r="M6" s="4"/>
       <c r="O6" s="1">
         <v>3</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
       <c r="R6" s="9">
         <v>-1</v>
       </c>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
-      <c r="V6" s="49"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
       <c r="W6" s="9">
         <v>-1</v>
       </c>
-      <c r="X6" s="52">
+      <c r="X6" s="51">
         <v>1</v>
       </c>
-      <c r="Y6" s="49"/>
+      <c r="Y6" s="48"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="48"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="59"/>
       <c r="M7" s="4"/>
       <c r="O7" s="1">
         <v>4</v>
       </c>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="52">
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="51">
         <v>3</v>
       </c>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49"/>
-      <c r="V7" s="49"/>
-      <c r="W7" s="52">
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="51">
         <v>1</v>
       </c>
-      <c r="X7" s="52">
+      <c r="X7" s="51">
         <v>1</v>
       </c>
-      <c r="Y7" s="49"/>
+      <c r="Y7" s="48"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="48"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="59"/>
       <c r="M8" s="4"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="49"/>
-      <c r="W8" s="49"/>
-      <c r="X8" s="49"/>
-      <c r="Y8" s="49"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="48"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="59"/>
       <c r="M9" s="4"/>
       <c r="O9" s="1">
         <v>6</v>
       </c>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="49"/>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="49"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="48"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="59"/>
       <c r="M10" s="4"/>
       <c r="O10" s="1">
         <v>7</v>
       </c>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="49"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="49"/>
-      <c r="V10" s="49"/>
-      <c r="W10" s="49"/>
-      <c r="X10" s="49"/>
-      <c r="Y10" s="49"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="48"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="59"/>
       <c r="M11" s="4"/>
       <c r="O11" s="1">
         <v>8</v>
       </c>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="49"/>
-      <c r="V11" s="49"/>
-      <c r="W11" s="49"/>
-      <c r="X11" s="49"/>
-      <c r="Y11" s="49"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="48"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="59"/>
       <c r="M12" s="4"/>
       <c r="O12" s="1">
         <v>9</v>
       </c>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="52">
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="51">
         <v>5</v>
       </c>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="49"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
-      <c r="X12" s="49"/>
-      <c r="Y12" s="49"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M13" s="4"/>
@@ -3638,7 +3653,7 @@
       <c r="W17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="X17" s="59" t="s">
+      <c r="X17" s="58" t="s">
         <v>8</v>
       </c>
       <c r="Y17" s="16" t="s">
@@ -3649,42 +3664,46 @@
       <c r="A18" s="1">
         <v>0</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="51">
         <v>8.94</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="54">
+      <c r="D18" s="53">
         <v>505.53</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="56">
+      <c r="E18" s="60"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="55">
         <v>295.70999999999998</v>
       </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="60"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="49"/>
+      <c r="K18" s="55">
+        <v>35.049999999999997</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="O18" s="1">
         <v>0</v>
       </c>
-      <c r="P18" s="54">
+      <c r="P18" s="53">
         <v>65</v>
       </c>
       <c r="Q18" s="9"/>
-      <c r="R18" s="54">
+      <c r="R18" s="53">
         <v>163</v>
       </c>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="57">
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="56">
         <v>187</v>
       </c>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="9"/>
       <c r="X18" s="13"/>
-      <c r="Y18" s="49"/>
+      <c r="Y18" s="51">
+        <v>146</v>
+      </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -3693,15 +3712,17 @@
       <c r="B19" s="46"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="56">
+      <c r="E19" s="60"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="55">
         <v>335.76</v>
       </c>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="60"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="49"/>
+      <c r="K19" s="55">
+        <v>740.08</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="O19" s="1">
         <v>1</v>
@@ -3709,15 +3730,17 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="49"/>
-      <c r="U19" s="57">
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="56">
         <v>262</v>
       </c>
-      <c r="V19" s="49"/>
-      <c r="W19" s="49"/>
+      <c r="V19" s="48"/>
+      <c r="W19" s="9"/>
       <c r="X19" s="13"/>
-      <c r="Y19" s="49"/>
+      <c r="Y19" s="51">
+        <v>185</v>
+      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -3725,36 +3748,36 @@
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="54">
+      <c r="D20" s="53">
         <v>258.99</v>
       </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="56">
+      <c r="E20" s="60"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="55">
         <v>885.99</v>
       </c>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="60"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="49"/>
+      <c r="K20" s="60"/>
       <c r="M20" s="4"/>
       <c r="O20" s="1">
         <v>2</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
-      <c r="R20" s="54">
+      <c r="R20" s="53">
         <v>136</v>
       </c>
-      <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
-      <c r="U20" s="57">
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="56">
         <v>364</v>
       </c>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="9"/>
       <c r="X20" s="13"/>
-      <c r="Y20" s="49"/>
+      <c r="Y20" s="9"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -3762,32 +3785,40 @@
       </c>
       <c r="B21" s="46"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="55">
+        <v>260.88</v>
+      </c>
       <c r="G21" s="9"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="56">
+      <c r="H21" s="48"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="55">
         <v>377.76</v>
       </c>
-      <c r="K21" s="49"/>
+      <c r="K21" s="55">
+        <v>56.53</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="O21" s="1">
         <v>3</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="51">
+        <v>68</v>
+      </c>
       <c r="U21" s="13"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="57">
+      <c r="V21" s="48"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="56">
         <v>153</v>
       </c>
-      <c r="Y21" s="49"/>
+      <c r="Y21" s="51">
+        <v>147</v>
+      </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="24">
@@ -3795,36 +3826,44 @@
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="54">
+      <c r="D22" s="53">
         <v>158.88</v>
       </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="56">
+      <c r="H22" s="49"/>
+      <c r="I22" s="55">
+        <v>1.22</v>
+      </c>
+      <c r="J22" s="55">
         <v>555.86</v>
       </c>
-      <c r="K22" s="50"/>
+      <c r="K22" s="55">
+        <v>214.47</v>
+      </c>
       <c r="M22" s="4"/>
       <c r="O22" s="1">
         <v>4</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
-      <c r="R22" s="54">
+      <c r="R22" s="53">
         <v>98</v>
       </c>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="50"/>
-      <c r="W22" s="50"/>
-      <c r="X22" s="57">
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="49"/>
+      <c r="W22" s="63">
+        <v>38</v>
+      </c>
+      <c r="X22" s="56">
         <v>133</v>
       </c>
-      <c r="Y22" s="50"/>
+      <c r="Y22" s="63">
+        <v>181</v>
+      </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
@@ -3832,36 +3871,36 @@
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="54">
+      <c r="D23" s="53">
         <v>385.23</v>
       </c>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="56">
+      <c r="E23" s="60"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="55">
         <v>507.3</v>
       </c>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="60"/>
       <c r="J23" s="10"/>
-      <c r="K23" s="50"/>
+      <c r="K23" s="60"/>
       <c r="M23" s="4"/>
       <c r="O23" s="1">
         <v>5</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
-      <c r="R23" s="54">
+      <c r="R23" s="53">
         <v>142</v>
       </c>
-      <c r="S23" s="49"/>
-      <c r="T23" s="49"/>
-      <c r="U23" s="57">
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="56">
         <v>241</v>
       </c>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="50"/>
+      <c r="V23" s="49"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="10"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
@@ -3869,40 +3908,44 @@
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="54">
+      <c r="D24" s="53">
         <v>266.64</v>
       </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="56">
+      <c r="E24" s="60"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="55">
         <v>215.17</v>
       </c>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="56">
+      <c r="H24" s="49"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="55">
         <v>124.26</v>
       </c>
-      <c r="K24" s="50"/>
+      <c r="K24" s="55">
+        <v>20.56</v>
+      </c>
       <c r="M24" s="4"/>
       <c r="O24" s="1">
         <v>6</v>
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
-      <c r="R24" s="54">
+      <c r="R24" s="53">
         <v>93</v>
       </c>
-      <c r="S24" s="49"/>
-      <c r="T24" s="49"/>
-      <c r="U24" s="57">
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="56">
         <v>154</v>
       </c>
-      <c r="V24" s="50"/>
-      <c r="W24" s="50"/>
-      <c r="X24" s="57">
+      <c r="V24" s="49"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="56">
         <v>118</v>
       </c>
-      <c r="Y24" s="50"/>
+      <c r="Y24" s="63">
+        <v>124</v>
+      </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
@@ -3910,40 +3953,44 @@
       </c>
       <c r="B25" s="47"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="54">
+      <c r="D25" s="53">
         <v>205.66</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="56">
+      <c r="E25" s="60"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="55">
         <v>366.21</v>
       </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="56">
+      <c r="H25" s="49"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="55">
         <v>710.67</v>
       </c>
-      <c r="K25" s="50"/>
+      <c r="K25" s="55">
+        <v>1.07</v>
+      </c>
       <c r="M25" s="4"/>
       <c r="O25" s="1">
         <v>7</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
-      <c r="R25" s="54">
+      <c r="R25" s="53">
         <v>111</v>
       </c>
-      <c r="S25" s="49"/>
-      <c r="T25" s="49"/>
-      <c r="U25" s="57">
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="56">
         <v>199</v>
       </c>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="57">
+      <c r="V25" s="49"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="56">
         <v>148</v>
       </c>
-      <c r="Y25" s="50"/>
+      <c r="Y25" s="63">
+        <v>113</v>
+      </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
@@ -3951,40 +3998,44 @@
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="54">
+      <c r="D26" s="53">
         <v>63.19</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="56">
+      <c r="E26" s="60"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="55">
         <v>4.3499999999999996</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="56">
+      <c r="H26" s="49"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="55">
         <v>829.02</v>
       </c>
-      <c r="K26" s="50"/>
+      <c r="K26" s="55">
+        <v>69.42</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="O26" s="1">
         <v>8</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
-      <c r="R26" s="54">
+      <c r="R26" s="53">
         <v>106</v>
       </c>
-      <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="57">
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="56">
         <v>78</v>
       </c>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
-      <c r="X26" s="57">
+      <c r="V26" s="49"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="56">
         <v>258</v>
       </c>
-      <c r="Y26" s="50"/>
+      <c r="Y26" s="63">
+        <v>94</v>
+      </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
@@ -3992,40 +4043,44 @@
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="54">
+      <c r="D27" s="53">
         <v>252.04</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="56">
+      <c r="E27" s="60"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="55">
         <v>347.65</v>
       </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="56">
+      <c r="H27" s="49"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="55">
         <v>850.38</v>
       </c>
-      <c r="K27" s="50"/>
+      <c r="K27" s="55">
+        <v>60.34</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="O27" s="1">
         <v>9</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
-      <c r="R27" s="54">
+      <c r="R27" s="53">
         <v>169</v>
       </c>
-      <c r="S27" s="49"/>
-      <c r="T27" s="49"/>
-      <c r="U27" s="57">
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="56">
         <v>187</v>
       </c>
-      <c r="V27" s="49"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="57">
+      <c r="V27" s="48"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="56">
         <v>358</v>
       </c>
-      <c r="Y27" s="49"/>
+      <c r="Y27" s="51">
+        <v>117</v>
+      </c>
     </row>
     <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
@@ -4039,7 +4094,7 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="53">
+      <c r="D28" s="52">
         <f t="shared" si="0"/>
         <v>262.02000000000004</v>
       </c>
@@ -4047,9 +4102,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="33" t="e">
+      <c r="F28" s="33">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>260.88</v>
       </c>
       <c r="G28" s="33">
         <f t="shared" si="0"/>
@@ -4059,17 +4114,17 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="33" t="e">
+      <c r="I28" s="33">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.22</v>
       </c>
       <c r="J28" s="33">
         <f t="shared" si="0"/>
         <v>574.65833333333342</v>
       </c>
-      <c r="K28" s="33" t="e">
+      <c r="K28" s="33">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>149.68999999999997</v>
       </c>
       <c r="M28" s="4"/>
     </row>
@@ -4093,9 +4148,9 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F29" s="21" t="e">
+      <c r="F29" s="21">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" si="1"/>
@@ -4105,17 +4160,17 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="21" t="e">
+      <c r="I29" s="21">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="J29" s="21">
         <f t="shared" si="1"/>
         <v>258.58669019735362</v>
       </c>
-      <c r="K29" s="21" t="e">
+      <c r="K29" s="21">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>231.23772194432291</v>
       </c>
       <c r="M29" s="4"/>
     </row>
@@ -4136,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="19">
         <v>8</v>
@@ -4145,17 +4200,17 @@
         <v>0</v>
       </c>
       <c r="I30" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="20">
         <v>6</v>
       </c>
-      <c r="K30" s="32">
-        <v>0</v>
+      <c r="K30" s="61">
+        <v>8</v>
       </c>
       <c r="L30" s="32">
         <f>SUM(B30:K30)</f>
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="M30" s="4"/>
     </row>
@@ -4195,14 +4250,14 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
       </c>
       <c r="M34" s="4"/>
       <c r="O34" s="17" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="P34" t="s">
         <v>17</v>
@@ -4283,40 +4338,44 @@
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="56">
+      <c r="D36" s="55">
         <v>4.5584199999999999</v>
       </c>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="56">
+      <c r="E36" s="55">
+        <v>1.0730500000000001</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="55">
         <v>0.12731100000000001</v>
       </c>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="56">
+      <c r="H36" s="48"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="55">
         <v>0.11088199999999999</v>
       </c>
-      <c r="K36" s="49"/>
+      <c r="K36" s="60"/>
       <c r="M36" s="4"/>
       <c r="O36" s="1">
         <v>0</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
-      <c r="R36" s="54">
+      <c r="R36" s="53">
         <v>142</v>
       </c>
-      <c r="S36" s="49"/>
-      <c r="T36" s="49"/>
-      <c r="U36" s="57">
+      <c r="S36" s="51">
+        <v>307</v>
+      </c>
+      <c r="T36" s="9"/>
+      <c r="U36" s="56">
         <v>187</v>
       </c>
-      <c r="V36" s="49"/>
-      <c r="W36" s="49"/>
-      <c r="X36" s="57">
+      <c r="V36" s="48"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="56">
         <v>153</v>
       </c>
-      <c r="Y36" s="49"/>
+      <c r="Y36" s="9"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -4324,40 +4383,44 @@
       </c>
       <c r="B37" s="46"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="56">
+      <c r="D37" s="55">
         <v>369.37900000000002</v>
       </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="56">
+      <c r="E37" s="55">
+        <v>1.17469</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="55">
         <v>0.137241</v>
       </c>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="56">
+      <c r="H37" s="48"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="55">
         <v>0.114484</v>
       </c>
-      <c r="K37" s="49"/>
+      <c r="K37" s="60"/>
       <c r="M37" s="4"/>
       <c r="O37" s="1">
         <v>1</v>
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
-      <c r="R37" s="54">
+      <c r="R37" s="53">
         <v>175</v>
       </c>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="57">
+      <c r="S37" s="51">
+        <v>532</v>
+      </c>
+      <c r="T37" s="9"/>
+      <c r="U37" s="56">
         <v>238</v>
       </c>
-      <c r="V37" s="49"/>
-      <c r="W37" s="49"/>
-      <c r="X37" s="57">
+      <c r="V37" s="48"/>
+      <c r="W37" s="9"/>
+      <c r="X37" s="56">
         <v>208</v>
       </c>
-      <c r="Y37" s="49"/>
+      <c r="Y37" s="9"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -4365,40 +4428,44 @@
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="56">
+      <c r="D38" s="55">
         <v>244.98400000000001</v>
       </c>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="56">
+      <c r="E38" s="55">
+        <v>1.0177700000000001</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="55">
         <v>0.145514</v>
       </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="56">
+      <c r="H38" s="48"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="55">
         <v>0.115649</v>
       </c>
-      <c r="K38" s="49"/>
+      <c r="K38" s="60"/>
       <c r="M38" s="4"/>
       <c r="O38" s="1">
         <v>2</v>
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
-      <c r="R38" s="54">
+      <c r="R38" s="53">
         <v>130</v>
       </c>
-      <c r="S38" s="49"/>
-      <c r="T38" s="49"/>
-      <c r="U38" s="57">
+      <c r="S38" s="51">
+        <v>346</v>
+      </c>
+      <c r="T38" s="9"/>
+      <c r="U38" s="56">
         <v>256</v>
       </c>
-      <c r="V38" s="49"/>
-      <c r="W38" s="49"/>
-      <c r="X38" s="57">
+      <c r="V38" s="48"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="56">
         <v>208</v>
       </c>
-      <c r="Y38" s="49"/>
+      <c r="Y38" s="9"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -4406,40 +4473,44 @@
       </c>
       <c r="B39" s="46"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="56">
+      <c r="D39" s="55">
         <v>88.552000000000007</v>
       </c>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="56">
+      <c r="E39" s="55">
+        <v>1.0498099999999999</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="55">
         <v>0.13156599999999999</v>
       </c>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="56">
+      <c r="H39" s="48"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="55">
         <v>8.8751200000000002E-2</v>
       </c>
-      <c r="K39" s="49"/>
+      <c r="K39" s="60"/>
       <c r="M39" s="4"/>
       <c r="O39" s="1">
         <v>3</v>
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="9"/>
-      <c r="R39" s="54">
+      <c r="R39" s="53">
         <v>134</v>
       </c>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="57">
+      <c r="S39" s="51">
+        <v>493</v>
+      </c>
+      <c r="T39" s="9"/>
+      <c r="U39" s="56">
         <v>208</v>
       </c>
-      <c r="V39" s="49"/>
-      <c r="W39" s="49"/>
-      <c r="X39" s="57">
+      <c r="V39" s="48"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="56">
         <v>148</v>
       </c>
-      <c r="Y39" s="49"/>
+      <c r="Y39" s="9"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
@@ -4447,40 +4518,44 @@
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="10"/>
-      <c r="D40" s="56">
+      <c r="D40" s="55">
         <v>3.7271200000000002</v>
       </c>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="56">
+      <c r="E40" s="55">
+        <v>1.1207400000000001</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="55">
         <v>0.16553699999999999</v>
       </c>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="56">
+      <c r="H40" s="49"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="55">
         <v>8.2298700000000002E-2</v>
       </c>
-      <c r="K40" s="50"/>
+      <c r="K40" s="60"/>
       <c r="M40" s="4"/>
       <c r="O40" s="1">
         <v>4</v>
       </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="9"/>
-      <c r="R40" s="54">
+      <c r="R40" s="53">
         <v>89</v>
       </c>
-      <c r="S40" s="49"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="57">
+      <c r="S40" s="51">
+        <v>445</v>
+      </c>
+      <c r="T40" s="10"/>
+      <c r="U40" s="56">
         <v>379</v>
       </c>
-      <c r="V40" s="50"/>
-      <c r="W40" s="50"/>
-      <c r="X40" s="57">
+      <c r="V40" s="49"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="56">
         <v>118</v>
       </c>
-      <c r="Y40" s="50"/>
+      <c r="Y40" s="10"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
@@ -4488,40 +4563,44 @@
       </c>
       <c r="B41" s="47"/>
       <c r="C41" s="10"/>
-      <c r="D41" s="56">
+      <c r="D41" s="55">
         <v>0.64394700000000005</v>
       </c>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="56">
+      <c r="E41" s="55">
+        <v>1.01284</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="55">
         <v>0.11219999999999999</v>
       </c>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="56">
+      <c r="H41" s="49"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="55">
         <v>0.11194</v>
       </c>
-      <c r="K41" s="50"/>
+      <c r="K41" s="60"/>
       <c r="M41" s="4"/>
       <c r="O41" s="1">
         <v>5</v>
       </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
-      <c r="R41" s="54">
+      <c r="R41" s="53">
         <v>103</v>
       </c>
-      <c r="S41" s="49"/>
-      <c r="T41" s="49"/>
-      <c r="U41" s="57">
+      <c r="S41" s="51">
+        <v>310</v>
+      </c>
+      <c r="T41" s="10"/>
+      <c r="U41" s="56">
         <v>199</v>
       </c>
-      <c r="V41" s="50"/>
-      <c r="W41" s="50"/>
-      <c r="X41" s="57">
+      <c r="V41" s="49"/>
+      <c r="W41" s="10"/>
+      <c r="X41" s="56">
         <v>148</v>
       </c>
-      <c r="Y41" s="50"/>
+      <c r="Y41" s="10"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="24">
@@ -4529,40 +4608,44 @@
       </c>
       <c r="B42" s="47"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="56">
+      <c r="D42" s="55">
         <v>0.41857299999999997</v>
       </c>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="56">
+      <c r="E42" s="55">
+        <v>1.3957900000000001</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="55">
         <v>0.108722</v>
       </c>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="56">
+      <c r="H42" s="49"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="55">
         <v>9.5584500000000003E-2</v>
       </c>
-      <c r="K42" s="50"/>
+      <c r="K42" s="60"/>
       <c r="M42" s="4"/>
       <c r="O42" s="1">
         <v>6</v>
       </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
-      <c r="R42" s="54">
+      <c r="R42" s="53">
         <v>93</v>
       </c>
-      <c r="S42" s="49"/>
-      <c r="T42" s="49"/>
-      <c r="U42" s="57">
+      <c r="S42" s="51">
+        <v>316</v>
+      </c>
+      <c r="T42" s="10"/>
+      <c r="U42" s="56">
         <v>154</v>
       </c>
-      <c r="V42" s="50"/>
-      <c r="W42" s="50"/>
-      <c r="X42" s="57">
+      <c r="V42" s="49"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="56">
         <v>98</v>
       </c>
-      <c r="Y42" s="50"/>
+      <c r="Y42" s="10"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="24">
@@ -4570,40 +4653,44 @@
       </c>
       <c r="B43" s="47"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="56">
+      <c r="D43" s="55">
         <v>0.33063700000000001</v>
       </c>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="56">
+      <c r="E43" s="55">
+        <v>1.03054</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="55">
         <v>0.106403</v>
       </c>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="56">
+      <c r="H43" s="49"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="55">
         <v>0.10772</v>
       </c>
-      <c r="K43" s="50"/>
+      <c r="K43" s="60"/>
       <c r="M43" s="4"/>
       <c r="O43" s="1">
         <v>7</v>
       </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="9"/>
-      <c r="R43" s="54">
+      <c r="R43" s="53">
         <v>99</v>
       </c>
-      <c r="S43" s="49"/>
-      <c r="T43" s="49"/>
-      <c r="U43" s="57">
+      <c r="S43" s="51">
+        <v>505</v>
+      </c>
+      <c r="T43" s="10"/>
+      <c r="U43" s="56">
         <v>199</v>
       </c>
-      <c r="V43" s="50"/>
-      <c r="W43" s="50"/>
-      <c r="X43" s="57">
+      <c r="V43" s="49"/>
+      <c r="W43" s="10"/>
+      <c r="X43" s="56">
         <v>138</v>
       </c>
-      <c r="Y43" s="50"/>
+      <c r="Y43" s="10"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="24">
@@ -4611,40 +4698,48 @@
       </c>
       <c r="B44" s="47"/>
       <c r="C44" s="10"/>
-      <c r="D44" s="56">
+      <c r="D44" s="55">
         <v>0.33985700000000002</v>
       </c>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="56">
+      <c r="E44" s="55">
+        <v>0.99276699999999996</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="55">
         <v>7.9479599999999997E-2</v>
       </c>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="56">
+      <c r="H44" s="49"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="55">
         <v>0.11412799999999999</v>
       </c>
-      <c r="K44" s="50"/>
+      <c r="K44" s="55">
+        <v>4.3423600000000002</v>
+      </c>
       <c r="M44" s="4"/>
       <c r="O44" s="1">
         <v>8</v>
       </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
-      <c r="R44" s="54">
+      <c r="R44" s="53">
         <v>106</v>
       </c>
-      <c r="S44" s="49"/>
-      <c r="T44" s="49"/>
-      <c r="U44" s="57">
+      <c r="S44" s="51">
+        <v>550</v>
+      </c>
+      <c r="T44" s="10"/>
+      <c r="U44" s="56">
         <v>72</v>
       </c>
-      <c r="V44" s="50"/>
-      <c r="W44" s="50"/>
-      <c r="X44" s="57">
+      <c r="V44" s="49"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="56">
         <v>258</v>
       </c>
-      <c r="Y44" s="50"/>
+      <c r="Y44" s="63">
+        <v>88</v>
+      </c>
     </row>
     <row r="45" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24">
@@ -4652,40 +4747,44 @@
       </c>
       <c r="B45" s="47"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="56">
+      <c r="D45" s="55">
         <v>0.54566099999999995</v>
       </c>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="56">
+      <c r="E45" s="55">
+        <v>0.94031600000000004</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="55">
         <v>7.1677299999999999E-2</v>
       </c>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="56">
+      <c r="H45" s="49"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="55">
         <v>0.15307000000000001</v>
       </c>
-      <c r="K45" s="50"/>
+      <c r="K45" s="60"/>
       <c r="M45" s="4"/>
       <c r="O45" s="1">
         <v>9</v>
       </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="9"/>
-      <c r="R45" s="54">
+      <c r="R45" s="53">
         <v>136</v>
       </c>
-      <c r="S45" s="49"/>
-      <c r="T45" s="49"/>
-      <c r="U45" s="57">
+      <c r="S45" s="51">
+        <v>289</v>
+      </c>
+      <c r="T45" s="10"/>
+      <c r="U45" s="56">
         <v>187</v>
       </c>
-      <c r="V45" s="49"/>
-      <c r="W45" s="49"/>
-      <c r="X45" s="57">
+      <c r="V45" s="48"/>
+      <c r="W45" s="9"/>
+      <c r="X45" s="56">
         <v>358</v>
       </c>
-      <c r="Y45" s="49"/>
+      <c r="Y45" s="9"/>
     </row>
     <row r="46" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
@@ -4703,9 +4802,9 @@
         <f t="shared" si="2"/>
         <v>71.347921500000012</v>
       </c>
-      <c r="E46" s="33" t="e">
+      <c r="E46" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.0808312999999998</v>
       </c>
       <c r="F46" s="33" t="e">
         <f t="shared" si="2"/>
@@ -4727,9 +4826,9 @@
         <f t="shared" si="2"/>
         <v>0.10945073999999999</v>
       </c>
-      <c r="K46" s="33" t="e">
+      <c r="K46" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>4.3423600000000002</v>
       </c>
       <c r="M46" s="4"/>
     </row>
@@ -4749,9 +4848,9 @@
         <f t="shared" si="3"/>
         <v>123.86685861614376</v>
       </c>
-      <c r="E47" s="21" t="e">
+      <c r="E47" s="21">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.12216899854222542</v>
       </c>
       <c r="F47" s="21" t="e">
         <f t="shared" si="3"/>
@@ -4773,9 +4872,9 @@
         <f t="shared" si="3"/>
         <v>1.8323443898197844E-2</v>
       </c>
-      <c r="K47" s="21" t="e">
+      <c r="K47" s="21">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M47" s="4"/>
     </row>
@@ -4793,7 +4892,7 @@
         <v>10</v>
       </c>
       <c r="E48" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F48" s="19">
         <v>0</v>
@@ -4810,12 +4909,12 @@
       <c r="J48" s="20">
         <v>10</v>
       </c>
-      <c r="K48" s="32">
-        <v>0</v>
+      <c r="K48" s="61">
+        <v>1</v>
       </c>
       <c r="L48" s="32">
         <f>SUM(B48:K48)</f>
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M48" s="4"/>
     </row>
@@ -4941,538 +5040,694 @@
       <c r="A54" s="1">
         <v>0</v>
       </c>
-      <c r="B54" s="56">
+      <c r="B54" s="55">
         <v>1.12389E-2</v>
       </c>
-      <c r="C54" s="56">
+      <c r="C54" s="55">
         <v>42.491300000000003</v>
       </c>
-      <c r="D54" s="56">
+      <c r="D54" s="55">
         <v>6.0726300000000002</v>
       </c>
-      <c r="E54" s="56">
+      <c r="E54" s="55">
         <v>18.004999999999999</v>
       </c>
-      <c r="F54" s="49"/>
-      <c r="G54" s="56">
+      <c r="F54" s="55">
+        <v>12.0899</v>
+      </c>
+      <c r="G54" s="55">
         <v>0.47940199999999999</v>
       </c>
-      <c r="H54" s="49"/>
-      <c r="I54" s="49">
+      <c r="H54" s="55">
+        <v>11.3604</v>
+      </c>
+      <c r="I54" s="55">
         <v>275.714</v>
       </c>
-      <c r="J54" s="49">
+      <c r="J54" s="55">
         <v>2.0734300000000001</v>
       </c>
-      <c r="K54" s="49"/>
+      <c r="K54" s="55">
+        <v>0.53345100000000001</v>
+      </c>
       <c r="M54" s="4"/>
       <c r="O54" s="1">
         <v>0</v>
       </c>
-      <c r="P54" s="57">
+      <c r="P54" s="56">
         <v>21</v>
       </c>
-      <c r="Q54" s="57">
+      <c r="Q54" s="56">
         <v>258</v>
       </c>
-      <c r="R54" s="49"/>
-      <c r="S54" s="49"/>
-      <c r="T54" s="49"/>
-      <c r="U54" s="49">
+      <c r="R54" s="56">
+        <v>178</v>
+      </c>
+      <c r="S54" s="56">
+        <v>355</v>
+      </c>
+      <c r="T54" s="56">
+        <v>350</v>
+      </c>
+      <c r="U54" s="56">
         <v>187</v>
       </c>
-      <c r="V54" s="49"/>
-      <c r="W54" s="49">
+      <c r="V54" s="56">
+        <v>173</v>
+      </c>
+      <c r="W54" s="56">
         <v>353</v>
       </c>
-      <c r="X54" s="49">
+      <c r="X54" s="56">
         <v>243</v>
       </c>
-      <c r="Y54" s="49"/>
+      <c r="Y54" s="56">
+        <v>140</v>
+      </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B55" s="56">
+      <c r="B55" s="55">
         <v>6.6536600000000004</v>
       </c>
-      <c r="C55" s="56">
+      <c r="C55" s="55">
         <v>30.741700000000002</v>
       </c>
-      <c r="D55" s="56">
+      <c r="D55" s="55">
         <v>10.238099999999999</v>
       </c>
-      <c r="E55" s="56">
+      <c r="E55" s="55">
         <v>44.814300000000003</v>
       </c>
-      <c r="F55" s="49"/>
-      <c r="G55" s="56">
+      <c r="F55" s="55">
+        <v>34.728400000000001</v>
+      </c>
+      <c r="G55" s="55">
         <v>0.38312600000000002</v>
       </c>
-      <c r="H55" s="49"/>
-      <c r="I55" s="49">
+      <c r="H55" s="55">
+        <v>13.377700000000001</v>
+      </c>
+      <c r="I55" s="55">
         <v>69.224100000000007</v>
       </c>
-      <c r="J55" s="49">
+      <c r="J55" s="55">
         <v>2.52434</v>
       </c>
-      <c r="K55" s="49"/>
+      <c r="K55" s="55">
+        <v>7.9037099999999999E-2</v>
+      </c>
       <c r="M55" s="4"/>
       <c r="O55" s="1">
         <v>1</v>
       </c>
-      <c r="P55" s="57">
+      <c r="P55" s="56">
         <v>121</v>
       </c>
-      <c r="Q55" s="57">
+      <c r="Q55" s="56">
         <v>208</v>
       </c>
-      <c r="R55" s="49"/>
-      <c r="S55" s="49"/>
-      <c r="T55" s="49"/>
-      <c r="U55" s="49">
+      <c r="R55" s="56">
+        <v>397</v>
+      </c>
+      <c r="S55" s="56">
+        <v>607</v>
+      </c>
+      <c r="T55" s="56">
+        <v>339</v>
+      </c>
+      <c r="U55" s="56">
         <v>238</v>
       </c>
-      <c r="V55" s="49"/>
-      <c r="W55" s="49">
+      <c r="V55" s="56">
+        <v>177</v>
+      </c>
+      <c r="W55" s="56">
         <v>208</v>
       </c>
-      <c r="X55" s="49">
+      <c r="X55" s="56">
         <v>223</v>
       </c>
-      <c r="Y55" s="49"/>
+      <c r="Y55" s="56">
+        <v>185</v>
+      </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2</v>
       </c>
-      <c r="B56" s="56">
+      <c r="B56" s="55">
         <v>0.16361800000000001</v>
       </c>
-      <c r="C56" s="56">
+      <c r="C56" s="55">
         <v>25.808399999999999</v>
       </c>
-      <c r="D56" s="56">
+      <c r="D56" s="55">
         <v>8.8827600000000007E-2</v>
       </c>
-      <c r="E56" s="56">
+      <c r="E56" s="55">
         <v>19.5749</v>
       </c>
-      <c r="F56" s="49"/>
-      <c r="G56" s="56">
+      <c r="F56" s="55">
+        <v>126.414</v>
+      </c>
+      <c r="G56" s="55">
         <v>0.50300400000000001</v>
       </c>
-      <c r="H56" s="49"/>
-      <c r="I56" s="49">
+      <c r="H56" s="55">
+        <v>10.3215</v>
+      </c>
+      <c r="I56" s="55">
         <v>14.936400000000001</v>
       </c>
-      <c r="J56" s="49">
+      <c r="J56" s="55">
         <v>1.3243</v>
       </c>
-      <c r="K56" s="49"/>
+      <c r="K56" s="55">
+        <v>0.94615700000000003</v>
+      </c>
       <c r="M56" s="4"/>
       <c r="O56" s="1">
         <v>2</v>
       </c>
-      <c r="P56" s="57">
+      <c r="P56" s="56">
         <v>42</v>
       </c>
-      <c r="Q56" s="57">
+      <c r="Q56" s="56">
         <v>175</v>
       </c>
-      <c r="R56" s="49"/>
-      <c r="S56" s="49"/>
-      <c r="T56" s="49"/>
-      <c r="U56" s="49">
+      <c r="R56" s="56">
+        <v>148</v>
+      </c>
+      <c r="S56" s="56">
+        <v>541</v>
+      </c>
+      <c r="T56" s="56">
+        <v>671</v>
+      </c>
+      <c r="U56" s="56">
         <v>256</v>
       </c>
-      <c r="V56" s="49"/>
-      <c r="W56" s="49">
+      <c r="V56" s="56">
+        <v>196</v>
+      </c>
+      <c r="W56" s="56">
         <v>148</v>
       </c>
-      <c r="X56" s="49">
+      <c r="X56" s="56">
         <v>258</v>
       </c>
-      <c r="Y56" s="49"/>
+      <c r="Y56" s="56">
+        <v>211</v>
+      </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>3</v>
       </c>
-      <c r="B57" s="56">
+      <c r="B57" s="55">
         <v>17.5992</v>
       </c>
-      <c r="C57" s="56">
+      <c r="C57" s="55">
         <v>49.455800000000004</v>
       </c>
-      <c r="D57" s="56">
+      <c r="D57" s="55">
         <v>9.7938299999999998</v>
       </c>
-      <c r="E57" s="56">
+      <c r="E57" s="55">
         <v>18.940899999999999</v>
       </c>
-      <c r="F57" s="49"/>
-      <c r="G57" s="56">
+      <c r="F57" s="55">
+        <v>1.05467</v>
+      </c>
+      <c r="G57" s="55">
         <v>0.54791000000000001</v>
       </c>
-      <c r="H57" s="49"/>
-      <c r="I57" s="49">
+      <c r="H57" s="55">
+        <v>12.2889</v>
+      </c>
+      <c r="I57" s="55">
         <v>0.18924099999999999</v>
       </c>
-      <c r="J57" s="49">
+      <c r="J57" s="55">
         <v>1.43055</v>
       </c>
-      <c r="K57" s="49"/>
+      <c r="K57" s="55">
+        <v>7.2814100000000007E-2</v>
+      </c>
       <c r="M57" s="4"/>
       <c r="O57" s="1">
         <v>3</v>
       </c>
-      <c r="P57" s="57">
+      <c r="P57" s="56">
         <v>82</v>
       </c>
-      <c r="Q57" s="57">
+      <c r="Q57" s="56">
         <v>349</v>
       </c>
-      <c r="R57" s="49"/>
-      <c r="S57" s="49"/>
-      <c r="T57" s="49"/>
-      <c r="U57" s="49">
+      <c r="R57" s="56">
+        <v>236</v>
+      </c>
+      <c r="S57" s="56">
+        <v>490</v>
+      </c>
+      <c r="T57" s="56">
+        <v>62</v>
+      </c>
+      <c r="U57" s="56">
         <v>208</v>
       </c>
-      <c r="V57" s="49"/>
-      <c r="W57" s="49">
+      <c r="V57" s="56">
+        <v>212</v>
+      </c>
+      <c r="W57" s="56">
         <v>57</v>
       </c>
-      <c r="X57" s="49">
+      <c r="X57" s="56">
         <v>253</v>
       </c>
-      <c r="Y57" s="49"/>
+      <c r="Y57" s="56">
+        <v>123</v>
+      </c>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
         <v>4</v>
       </c>
-      <c r="B58" s="56">
+      <c r="B58" s="55">
         <v>29.069099999999999</v>
       </c>
-      <c r="C58" s="56">
+      <c r="C58" s="55">
         <v>2.6156700000000002</v>
       </c>
-      <c r="D58" s="56">
+      <c r="D58" s="55">
         <v>6.22377</v>
       </c>
-      <c r="E58" s="56">
+      <c r="E58" s="55">
         <v>13.1508</v>
       </c>
-      <c r="F58" s="50"/>
-      <c r="G58" s="56">
+      <c r="F58" s="60"/>
+      <c r="G58" s="55">
         <v>0.70573300000000005</v>
       </c>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50">
+      <c r="H58" s="55">
+        <v>0.52202000000000004</v>
+      </c>
+      <c r="I58" s="55">
         <v>6.9745100000000004E-2</v>
       </c>
-      <c r="J58" s="50">
+      <c r="J58" s="55">
         <v>0.73257499999999998</v>
       </c>
-      <c r="K58" s="50"/>
+      <c r="K58" s="55">
+        <v>8.7135099999999993E-2</v>
+      </c>
       <c r="M58" s="4"/>
       <c r="O58" s="1">
         <v>4</v>
       </c>
-      <c r="P58" s="57">
+      <c r="P58" s="56">
         <v>137</v>
       </c>
-      <c r="Q58" s="57">
+      <c r="Q58" s="56">
         <v>102</v>
       </c>
-      <c r="R58" s="49"/>
-      <c r="S58" s="49"/>
-      <c r="T58" s="49"/>
-      <c r="U58" s="49">
+      <c r="R58" s="56">
+        <v>158</v>
+      </c>
+      <c r="S58" s="56">
+        <v>472</v>
+      </c>
+      <c r="T58" s="62"/>
+      <c r="U58" s="56">
         <v>379</v>
       </c>
-      <c r="V58" s="50"/>
-      <c r="W58" s="50">
+      <c r="V58" s="56">
+        <v>86</v>
+      </c>
+      <c r="W58" s="56">
         <v>29</v>
       </c>
-      <c r="X58" s="50">
+      <c r="X58" s="56">
         <v>133</v>
       </c>
-      <c r="Y58" s="50"/>
+      <c r="Y58" s="56">
+        <v>172</v>
+      </c>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="24">
         <v>5</v>
       </c>
-      <c r="B59" s="56">
+      <c r="B59" s="55">
         <v>0.132461</v>
       </c>
-      <c r="C59" s="56">
+      <c r="C59" s="55">
         <v>15.929600000000001</v>
       </c>
-      <c r="D59" s="56">
+      <c r="D59" s="55">
         <v>4.43478E-2</v>
       </c>
-      <c r="E59" s="56">
+      <c r="E59" s="55">
         <v>35.987299999999998</v>
       </c>
-      <c r="F59" s="50"/>
-      <c r="G59" s="56">
+      <c r="F59" s="55">
+        <v>18.217300000000002</v>
+      </c>
+      <c r="G59" s="55">
         <v>0.43384499999999998</v>
       </c>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50">
+      <c r="H59" s="55">
+        <v>12.176</v>
+      </c>
+      <c r="I59" s="55">
         <v>246.53399999999999</v>
       </c>
-      <c r="J59" s="50">
+      <c r="J59" s="55">
         <v>0.83743500000000004</v>
       </c>
-      <c r="K59" s="50"/>
+      <c r="K59" s="55">
+        <v>5.3616999999999998E-2</v>
+      </c>
       <c r="M59" s="4"/>
       <c r="O59" s="1">
         <v>5</v>
       </c>
-      <c r="P59" s="57">
+      <c r="P59" s="56">
         <v>77</v>
       </c>
-      <c r="Q59" s="57">
+      <c r="Q59" s="56">
         <v>163</v>
       </c>
-      <c r="R59" s="49"/>
-      <c r="S59" s="49"/>
-      <c r="T59" s="49"/>
-      <c r="U59" s="49">
+      <c r="R59" s="56">
+        <v>148</v>
+      </c>
+      <c r="S59" s="56">
+        <v>460</v>
+      </c>
+      <c r="T59" s="56">
+        <v>181</v>
+      </c>
+      <c r="U59" s="56">
         <v>199</v>
       </c>
-      <c r="V59" s="50"/>
-      <c r="W59" s="50">
+      <c r="V59" s="56">
+        <v>136</v>
+      </c>
+      <c r="W59" s="56">
         <v>193</v>
       </c>
-      <c r="X59" s="50">
+      <c r="X59" s="56">
         <v>163</v>
       </c>
-      <c r="Y59" s="50"/>
+      <c r="Y59" s="56">
+        <v>157</v>
+      </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="24">
         <v>6</v>
       </c>
-      <c r="B60" s="56">
+      <c r="B60" s="55">
         <v>40.249200000000002</v>
       </c>
-      <c r="C60" s="56">
+      <c r="C60" s="55">
         <v>23.0289</v>
       </c>
-      <c r="D60" s="56">
+      <c r="D60" s="55">
         <v>4.2488100000000001E-2</v>
       </c>
-      <c r="E60" s="56">
+      <c r="E60" s="55">
         <v>21.556999999999999</v>
       </c>
-      <c r="F60" s="50"/>
-      <c r="G60" s="56">
+      <c r="F60" s="55">
+        <v>1.8813</v>
+      </c>
+      <c r="G60" s="55">
         <v>0.44375300000000001</v>
       </c>
-      <c r="H60" s="50"/>
-      <c r="I60" s="50">
+      <c r="H60" s="55">
+        <v>19.398</v>
+      </c>
+      <c r="I60" s="55">
         <v>130.51599999999999</v>
       </c>
-      <c r="J60" s="50">
+      <c r="J60" s="55">
         <v>1.39022</v>
       </c>
-      <c r="K60" s="50"/>
+      <c r="K60" s="55">
+        <v>5.9117000000000003E-2</v>
+      </c>
       <c r="M60" s="4"/>
       <c r="O60" s="1">
         <v>6</v>
       </c>
-      <c r="P60" s="57">
+      <c r="P60" s="56">
         <v>327</v>
       </c>
-      <c r="Q60" s="57">
+      <c r="Q60" s="56">
         <v>203</v>
       </c>
-      <c r="R60" s="49"/>
-      <c r="S60" s="49"/>
-      <c r="T60" s="49"/>
-      <c r="U60" s="49">
+      <c r="R60" s="56">
+        <v>135</v>
+      </c>
+      <c r="S60" s="56">
+        <v>343</v>
+      </c>
+      <c r="T60" s="56">
+        <v>120</v>
+      </c>
+      <c r="U60" s="56">
         <v>154</v>
       </c>
-      <c r="V60" s="50"/>
-      <c r="W60" s="50">
+      <c r="V60" s="56">
+        <v>173</v>
+      </c>
+      <c r="W60" s="56">
         <v>308</v>
       </c>
-      <c r="X60" s="50">
+      <c r="X60" s="56">
         <v>128</v>
       </c>
-      <c r="Y60" s="50"/>
+      <c r="Y60" s="56">
+        <v>136</v>
+      </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="24">
         <v>7</v>
       </c>
-      <c r="B61" s="56">
+      <c r="B61" s="55">
         <v>512.66999999999996</v>
       </c>
-      <c r="C61" s="56">
+      <c r="C61" s="55">
         <v>11.9932</v>
       </c>
-      <c r="D61" s="56">
+      <c r="D61" s="55">
         <v>4.3576899999999998</v>
       </c>
-      <c r="E61" s="56">
+      <c r="E61" s="55">
         <v>24.514700000000001</v>
       </c>
-      <c r="F61" s="50"/>
-      <c r="G61" s="56">
+      <c r="F61" s="55">
+        <v>21.223299999999998</v>
+      </c>
+      <c r="G61" s="55">
         <v>0.37591000000000002</v>
       </c>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50">
+      <c r="H61" s="55">
+        <v>11.274699999999999</v>
+      </c>
+      <c r="I61" s="55">
         <v>10.2547</v>
       </c>
-      <c r="J61" s="50">
+      <c r="J61" s="55">
         <v>0.81820199999999998</v>
       </c>
-      <c r="K61" s="50"/>
+      <c r="K61" s="55">
+        <v>4.54711E-2</v>
+      </c>
       <c r="M61" s="4"/>
       <c r="O61" s="1">
         <v>7</v>
       </c>
-      <c r="P61" s="57">
+      <c r="P61" s="56">
         <v>336</v>
       </c>
-      <c r="Q61" s="57">
+      <c r="Q61" s="56">
         <v>227</v>
       </c>
-      <c r="R61" s="49"/>
-      <c r="S61" s="49"/>
-      <c r="T61" s="49"/>
-      <c r="U61" s="49">
+      <c r="R61" s="56">
+        <v>99</v>
+      </c>
+      <c r="S61" s="56">
+        <v>526</v>
+      </c>
+      <c r="T61" s="56">
+        <v>165</v>
+      </c>
+      <c r="U61" s="56">
         <v>199</v>
       </c>
-      <c r="V61" s="50"/>
-      <c r="W61" s="50">
+      <c r="V61" s="56">
+        <v>191</v>
+      </c>
+      <c r="W61" s="56">
         <v>212</v>
       </c>
-      <c r="X61" s="50">
+      <c r="X61" s="56">
         <v>148</v>
       </c>
-      <c r="Y61" s="50"/>
+      <c r="Y61" s="56">
+        <v>191</v>
+      </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>8</v>
       </c>
-      <c r="B62" s="56">
+      <c r="B62" s="55">
         <v>20.802</v>
       </c>
-      <c r="C62" s="56">
+      <c r="C62" s="55">
         <v>12.725</v>
       </c>
-      <c r="D62" s="56">
+      <c r="D62" s="55">
         <v>3.2014999999999998</v>
       </c>
-      <c r="E62" s="56">
+      <c r="E62" s="55">
         <v>11.315799999999999</v>
       </c>
-      <c r="F62" s="50"/>
-      <c r="G62" s="56">
+      <c r="F62" s="55">
+        <v>3.78572</v>
+      </c>
+      <c r="G62" s="55">
         <v>0.30377300000000002</v>
       </c>
-      <c r="H62" s="50"/>
-      <c r="I62" s="50">
+      <c r="H62" s="55">
+        <v>11.4245</v>
+      </c>
+      <c r="I62" s="55">
         <v>27.8551</v>
       </c>
-      <c r="J62" s="50">
+      <c r="J62" s="55">
         <v>1.5124599999999999</v>
       </c>
-      <c r="K62" s="50"/>
+      <c r="K62" s="55">
+        <v>0.27271699999999999</v>
+      </c>
       <c r="M62" s="4"/>
       <c r="O62" s="1">
         <v>8</v>
       </c>
-      <c r="P62" s="57">
+      <c r="P62" s="56">
         <v>227</v>
       </c>
-      <c r="Q62" s="57">
+      <c r="Q62" s="56">
         <v>254</v>
       </c>
-      <c r="R62" s="49"/>
-      <c r="S62" s="49"/>
-      <c r="T62" s="49"/>
-      <c r="U62" s="49">
+      <c r="R62" s="56">
+        <v>139</v>
+      </c>
+      <c r="S62" s="56">
+        <v>559</v>
+      </c>
+      <c r="T62" s="56">
+        <v>230</v>
+      </c>
+      <c r="U62" s="56">
         <v>72</v>
       </c>
-      <c r="V62" s="50"/>
-      <c r="W62" s="50">
+      <c r="V62" s="56">
+        <v>211</v>
+      </c>
+      <c r="W62" s="56">
         <v>207</v>
       </c>
-      <c r="X62" s="50">
+      <c r="X62" s="56">
         <v>288</v>
       </c>
-      <c r="Y62" s="50"/>
+      <c r="Y62" s="56">
+        <v>112</v>
+      </c>
     </row>
     <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="24">
         <v>9</v>
       </c>
-      <c r="B63" s="56">
+      <c r="B63" s="55">
         <v>565.20100000000002</v>
       </c>
-      <c r="C63" s="56">
+      <c r="C63" s="55">
         <v>14.2669</v>
       </c>
-      <c r="D63" s="56">
+      <c r="D63" s="55">
         <v>4.6919500000000003</v>
       </c>
-      <c r="E63" s="56">
+      <c r="E63" s="55">
         <v>12.3293</v>
       </c>
-      <c r="F63" s="50"/>
-      <c r="G63" s="56">
+      <c r="F63" s="55">
+        <v>8.7304200000000005</v>
+      </c>
+      <c r="G63" s="55">
         <v>0.38303500000000001</v>
       </c>
-      <c r="H63" s="50"/>
-      <c r="I63" s="50">
+      <c r="H63" s="55">
+        <v>16.6342</v>
+      </c>
+      <c r="I63" s="55">
         <v>12.4886</v>
       </c>
-      <c r="J63" s="50">
+      <c r="J63" s="55">
         <v>2.1301299999999999</v>
       </c>
-      <c r="K63" s="50"/>
+      <c r="K63" s="55">
+        <v>3.8875E-2</v>
+      </c>
       <c r="M63" s="4"/>
       <c r="O63" s="1">
         <v>9</v>
       </c>
-      <c r="P63" s="57">
+      <c r="P63" s="56">
         <v>313</v>
       </c>
-      <c r="Q63" s="57">
+      <c r="Q63" s="56">
         <v>175</v>
       </c>
-      <c r="R63" s="49"/>
-      <c r="S63" s="49"/>
-      <c r="T63" s="49"/>
-      <c r="U63" s="49">
+      <c r="R63" s="56">
+        <v>196</v>
+      </c>
+      <c r="S63" s="56">
+        <v>367</v>
+      </c>
+      <c r="T63" s="56">
+        <v>208</v>
+      </c>
+      <c r="U63" s="56">
         <v>187</v>
       </c>
-      <c r="V63" s="49"/>
-      <c r="W63" s="49">
+      <c r="V63" s="56">
+        <v>176</v>
+      </c>
+      <c r="W63" s="56">
         <v>330</v>
       </c>
-      <c r="X63" s="49">
+      <c r="X63" s="56">
         <v>343</v>
       </c>
-      <c r="Y63" s="49"/>
+      <c r="Y63" s="56">
+        <v>132</v>
+      </c>
     </row>
     <row r="64" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B64" s="33">
-        <f t="shared" ref="B64:K64" si="4">AVERAGE(B54:B63)</f>
+        <f t="shared" ref="B64:J64" si="4">AVERAGE(B54:B63)</f>
         <v>119.25514779</v>
       </c>
       <c r="C64" s="34">
@@ -5487,17 +5742,17 @@
         <f t="shared" si="4"/>
         <v>22.018999999999998</v>
       </c>
-      <c r="F64" s="33" t="e">
+      <c r="F64" s="33">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>25.347223333333332</v>
       </c>
       <c r="G64" s="33">
         <f t="shared" si="4"/>
         <v>0.45594909999999994</v>
       </c>
-      <c r="H64" s="33" t="e">
+      <c r="H64" s="33">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>11.877791999999999</v>
       </c>
       <c r="I64" s="33">
         <f t="shared" si="4"/>
@@ -5507,9 +5762,9 @@
         <f t="shared" si="4"/>
         <v>1.4773641999999998</v>
       </c>
-      <c r="K64" s="33" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="K64" s="33">
+        <f>AVERAGE(K54:K63)</f>
+        <v>0.21883914000000004</v>
       </c>
       <c r="M64" s="4"/>
     </row>
@@ -5518,7 +5773,7 @@
         <v>20</v>
       </c>
       <c r="B65" s="21">
-        <f t="shared" ref="B65:K65" si="5">_xlfn.STDEV.P(B54:B63)</f>
+        <f t="shared" ref="B65:J65" si="5">_xlfn.STDEV.P(B54:B63)</f>
         <v>210.55084371985251</v>
       </c>
       <c r="C65" s="21">
@@ -5533,17 +5788,17 @@
         <f t="shared" si="5"/>
         <v>10.197231670703582</v>
       </c>
-      <c r="F65" s="21" t="e">
+      <c r="F65" s="21">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>37.160153806276007</v>
       </c>
       <c r="G65" s="21">
         <f t="shared" si="5"/>
         <v>0.10697375139018937</v>
       </c>
-      <c r="H65" s="21" t="e">
+      <c r="H65" s="21">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>4.6249010564309394</v>
       </c>
       <c r="I65" s="21">
         <f t="shared" si="5"/>
@@ -5553,9 +5808,9 @@
         <f t="shared" si="5"/>
         <v>0.57538831567365101</v>
       </c>
-      <c r="K65" s="21" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+      <c r="K65" s="21">
+        <f>_xlfn.STDEV.P(K54:K63)</f>
+        <v>0.28360918163998916</v>
       </c>
       <c r="M65" s="4"/>
     </row>
@@ -5576,26 +5831,26 @@
         <v>10</v>
       </c>
       <c r="F66" s="19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G66" s="19">
         <v>10</v>
       </c>
       <c r="H66" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I66" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J66" s="20">
-        <v>0</v>
-      </c>
-      <c r="K66" s="32">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="K66" s="61">
+        <v>10</v>
       </c>
       <c r="L66" s="32">
         <f>SUM(B66:K66)</f>
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="M66" s="4"/>
     </row>

</xml_diff>

<commit_message>
Fixing bug from previous commit (zenpuzzle VGDL modified)
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A7F7CF-D072-4CA1-9C51-6363A2EFF550}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37BD44B-4243-4FF5-984D-17471AD65567}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="42">
   <si>
     <t>GVGAI level</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>FD (A*)</t>
+  </si>
+  <si>
+    <t>Loops</t>
   </si>
 </sst>
 </file>
@@ -3103,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
   <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3253,8 +3256,8 @@
       <c r="V3" s="48"/>
       <c r="W3" s="48"/>
       <c r="X3" s="48"/>
-      <c r="Y3" s="9">
-        <v>-1</v>
+      <c r="Y3" s="51">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -3288,9 +3291,7 @@
       <c r="V4" s="48"/>
       <c r="W4" s="48"/>
       <c r="X4" s="48"/>
-      <c r="Y4" s="9">
-        <v>-1</v>
-      </c>
+      <c r="Y4" s="48"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -3347,7 +3348,9 @@
         <v>-1</v>
       </c>
       <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
+      <c r="T6" s="48" t="s">
+        <v>41</v>
+      </c>
       <c r="U6" s="48"/>
       <c r="V6" s="48"/>
       <c r="W6" s="9">
@@ -3478,7 +3481,7 @@
       <c r="V10" s="48"/>
       <c r="W10" s="48"/>
       <c r="X10" s="48"/>
-      <c r="Y10" s="48">
+      <c r="Y10" s="51">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug in bounceForward, killIfOtherHasMore and ChipsVGDL
Fixed
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655E6188-0C2F-4E68-ABDE-45F263ADBA0D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB82DC9-F293-4499-BEAC-DE92D9DC2D7E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="42">
   <si>
     <t>GVGAI level</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>FD (A*)</t>
-  </si>
-  <si>
-    <t>Loops</t>
   </si>
   <si>
     <t>Saarplan</t>
@@ -553,14 +550,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3109,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,9 +3348,7 @@
         <v>-1</v>
       </c>
       <c r="S6" s="48"/>
-      <c r="T6" s="48" t="s">
-        <v>41</v>
-      </c>
+      <c r="T6" s="48"/>
       <c r="U6" s="48"/>
       <c r="V6" s="48"/>
       <c r="W6" s="9">
@@ -3700,7 +3695,7 @@
         <v>163</v>
       </c>
       <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
+      <c r="T18" s="42"/>
       <c r="U18" s="55">
         <v>187</v>
       </c>
@@ -3737,7 +3732,7 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="T19" s="42"/>
       <c r="U19" s="55">
         <v>262</v>
       </c>
@@ -3776,7 +3771,7 @@
         <v>136</v>
       </c>
       <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+      <c r="T20" s="42"/>
       <c r="U20" s="55">
         <v>364</v>
       </c>
@@ -3813,7 +3808,7 @@
       <c r="Q21" s="9"/>
       <c r="R21" s="53"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="50">
+      <c r="T21" s="42">
         <v>68</v>
       </c>
       <c r="U21" s="13"/>
@@ -3858,16 +3853,16 @@
         <v>98</v>
       </c>
       <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+      <c r="T22" s="42"/>
       <c r="U22" s="56"/>
       <c r="V22" s="10"/>
-      <c r="W22" s="62">
+      <c r="W22" s="61">
         <v>38</v>
       </c>
       <c r="X22" s="55">
         <v>133</v>
       </c>
-      <c r="Y22" s="62">
+      <c r="Y22" s="61">
         <v>181</v>
       </c>
     </row>
@@ -3899,7 +3894,7 @@
         <v>142</v>
       </c>
       <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
+      <c r="T23" s="42"/>
       <c r="U23" s="55">
         <v>241</v>
       </c>
@@ -3940,7 +3935,7 @@
         <v>93</v>
       </c>
       <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
+      <c r="T24" s="42"/>
       <c r="U24" s="55">
         <v>154</v>
       </c>
@@ -3949,7 +3944,7 @@
       <c r="X24" s="55">
         <v>118</v>
       </c>
-      <c r="Y24" s="62">
+      <c r="Y24" s="61">
         <v>124</v>
       </c>
     </row>
@@ -3985,7 +3980,7 @@
         <v>111</v>
       </c>
       <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
+      <c r="T25" s="42"/>
       <c r="U25" s="55">
         <v>199</v>
       </c>
@@ -3994,7 +3989,7 @@
       <c r="X25" s="55">
         <v>148</v>
       </c>
-      <c r="Y25" s="62">
+      <c r="Y25" s="61">
         <v>113</v>
       </c>
     </row>
@@ -4030,7 +4025,7 @@
         <v>106</v>
       </c>
       <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
+      <c r="T26" s="42"/>
       <c r="U26" s="55">
         <v>78</v>
       </c>
@@ -4039,7 +4034,7 @@
       <c r="X26" s="55">
         <v>258</v>
       </c>
-      <c r="Y26" s="62">
+      <c r="Y26" s="61">
         <v>94</v>
       </c>
     </row>
@@ -4075,7 +4070,7 @@
         <v>169</v>
       </c>
       <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+      <c r="T27" s="42"/>
       <c r="U27" s="55">
         <v>187</v>
       </c>
@@ -4372,7 +4367,7 @@
       <c r="S36" s="50">
         <v>307</v>
       </c>
-      <c r="T36" s="9"/>
+      <c r="T36" s="42"/>
       <c r="U36" s="55">
         <v>187</v>
       </c>
@@ -4417,7 +4412,7 @@
       <c r="S37" s="50">
         <v>532</v>
       </c>
-      <c r="T37" s="9"/>
+      <c r="T37" s="42"/>
       <c r="U37" s="55">
         <v>238</v>
       </c>
@@ -4462,7 +4457,7 @@
       <c r="S38" s="50">
         <v>346</v>
       </c>
-      <c r="T38" s="9"/>
+      <c r="T38" s="42"/>
       <c r="U38" s="55">
         <v>256</v>
       </c>
@@ -4507,7 +4502,7 @@
       <c r="S39" s="50">
         <v>493</v>
       </c>
-      <c r="T39" s="9"/>
+      <c r="T39" s="42"/>
       <c r="U39" s="55">
         <v>208</v>
       </c>
@@ -4552,7 +4547,7 @@
       <c r="S40" s="50">
         <v>445</v>
       </c>
-      <c r="T40" s="10"/>
+      <c r="T40" s="43"/>
       <c r="U40" s="55">
         <v>379</v>
       </c>
@@ -4597,7 +4592,7 @@
       <c r="S41" s="50">
         <v>310</v>
       </c>
-      <c r="T41" s="10"/>
+      <c r="T41" s="43"/>
       <c r="U41" s="55">
         <v>199</v>
       </c>
@@ -4642,7 +4637,7 @@
       <c r="S42" s="50">
         <v>316</v>
       </c>
-      <c r="T42" s="10"/>
+      <c r="T42" s="43"/>
       <c r="U42" s="55">
         <v>154</v>
       </c>
@@ -4687,7 +4682,7 @@
       <c r="S43" s="50">
         <v>505</v>
       </c>
-      <c r="T43" s="10"/>
+      <c r="T43" s="43"/>
       <c r="U43" s="55">
         <v>199</v>
       </c>
@@ -4734,7 +4729,7 @@
       <c r="S44" s="50">
         <v>550</v>
       </c>
-      <c r="T44" s="10"/>
+      <c r="T44" s="43"/>
       <c r="U44" s="55">
         <v>72</v>
       </c>
@@ -4743,7 +4738,7 @@
       <c r="X44" s="55">
         <v>258</v>
       </c>
-      <c r="Y44" s="62">
+      <c r="Y44" s="61">
         <v>88</v>
       </c>
     </row>
@@ -4781,7 +4776,7 @@
       <c r="S45" s="50">
         <v>289</v>
       </c>
-      <c r="T45" s="9"/>
+      <c r="T45" s="42"/>
       <c r="U45" s="55">
         <v>187</v>
       </c>
@@ -5092,7 +5087,7 @@
       <c r="S54" s="55">
         <v>355</v>
       </c>
-      <c r="T54" s="55">
+      <c r="T54" s="63">
         <v>350</v>
       </c>
       <c r="U54" s="55">
@@ -5161,7 +5156,7 @@
       <c r="S55" s="55">
         <v>607</v>
       </c>
-      <c r="T55" s="55">
+      <c r="T55" s="63">
         <v>339</v>
       </c>
       <c r="U55" s="55">
@@ -5230,7 +5225,7 @@
       <c r="S56" s="55">
         <v>541</v>
       </c>
-      <c r="T56" s="55">
+      <c r="T56" s="63">
         <v>671</v>
       </c>
       <c r="U56" s="55">
@@ -5299,7 +5294,7 @@
       <c r="S57" s="55">
         <v>490</v>
       </c>
-      <c r="T57" s="55">
+      <c r="T57" s="63">
         <v>62</v>
       </c>
       <c r="U57" s="55">
@@ -5366,7 +5361,7 @@
       <c r="S58" s="55">
         <v>472</v>
       </c>
-      <c r="T58" s="61"/>
+      <c r="T58" s="63"/>
       <c r="U58" s="55">
         <v>379</v>
       </c>
@@ -5433,7 +5428,7 @@
       <c r="S59" s="55">
         <v>460</v>
       </c>
-      <c r="T59" s="55">
+      <c r="T59" s="63">
         <v>181</v>
       </c>
       <c r="U59" s="55">
@@ -5502,7 +5497,7 @@
       <c r="S60" s="55">
         <v>343</v>
       </c>
-      <c r="T60" s="55">
+      <c r="T60" s="63">
         <v>120</v>
       </c>
       <c r="U60" s="55">
@@ -5571,7 +5566,7 @@
       <c r="S61" s="55">
         <v>526</v>
       </c>
-      <c r="T61" s="55">
+      <c r="T61" s="63">
         <v>165</v>
       </c>
       <c r="U61" s="55">
@@ -5640,7 +5635,7 @@
       <c r="S62" s="55">
         <v>559</v>
       </c>
-      <c r="T62" s="55">
+      <c r="T62" s="63">
         <v>230</v>
       </c>
       <c r="U62" s="55">
@@ -5709,7 +5704,7 @@
       <c r="S63" s="55">
         <v>367</v>
       </c>
-      <c r="T63" s="55">
+      <c r="T63" s="63">
         <v>208</v>
       </c>
       <c r="U63" s="55">
@@ -5896,14 +5891,14 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
       </c>
       <c r="M70" s="4"/>
       <c r="O70" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P70" t="s">
         <v>17</v>
@@ -6170,11 +6165,11 @@
       <c r="E76" s="54">
         <v>4.2425199999999998</v>
       </c>
-      <c r="F76" s="63"/>
+      <c r="F76" s="62"/>
       <c r="G76" s="54">
         <v>0.19906299999999999</v>
       </c>
-      <c r="H76" s="63"/>
+      <c r="H76" s="62"/>
       <c r="I76" s="59"/>
       <c r="J76" s="54">
         <v>5.1220700000000001E-2</v>
@@ -6192,11 +6187,11 @@
       <c r="S76" s="55">
         <v>481</v>
       </c>
-      <c r="T76" s="63"/>
+      <c r="T76" s="62"/>
       <c r="U76" s="55">
         <v>379</v>
       </c>
-      <c r="V76" s="63"/>
+      <c r="V76" s="62"/>
       <c r="W76" s="10"/>
       <c r="X76" s="55">
         <v>118</v>
@@ -6215,11 +6210,11 @@
       <c r="E77" s="54">
         <v>4.8396100000000004</v>
       </c>
-      <c r="F77" s="63"/>
+      <c r="F77" s="62"/>
       <c r="G77" s="54">
         <v>0.10667500000000001</v>
       </c>
-      <c r="H77" s="63"/>
+      <c r="H77" s="62"/>
       <c r="I77" s="59"/>
       <c r="J77" s="54">
         <v>8.2027600000000006E-2</v>
@@ -6237,11 +6232,11 @@
       <c r="S77" s="55">
         <v>601</v>
       </c>
-      <c r="T77" s="63"/>
+      <c r="T77" s="62"/>
       <c r="U77" s="55">
         <v>241</v>
       </c>
-      <c r="V77" s="63"/>
+      <c r="V77" s="62"/>
       <c r="W77" s="10"/>
       <c r="X77" s="55">
         <v>148</v>
@@ -6260,11 +6255,11 @@
       <c r="E78" s="54">
         <v>3.2199</v>
       </c>
-      <c r="F78" s="63"/>
+      <c r="F78" s="62"/>
       <c r="G78" s="54">
         <v>0.106572</v>
       </c>
-      <c r="H78" s="63"/>
+      <c r="H78" s="62"/>
       <c r="I78" s="59"/>
       <c r="J78" s="54">
         <v>5.05064E-2</v>
@@ -6282,11 +6277,11 @@
       <c r="S78" s="55">
         <v>328</v>
       </c>
-      <c r="T78" s="63"/>
+      <c r="T78" s="62"/>
       <c r="U78" s="55">
         <v>154</v>
       </c>
-      <c r="V78" s="63"/>
+      <c r="V78" s="62"/>
       <c r="W78" s="10"/>
       <c r="X78" s="55">
         <v>98</v>
@@ -6305,11 +6300,11 @@
       <c r="E79" s="54">
         <v>3.1267800000000001</v>
       </c>
-      <c r="F79" s="63"/>
+      <c r="F79" s="62"/>
       <c r="G79" s="54">
         <v>8.7227299999999994E-2</v>
       </c>
-      <c r="H79" s="63"/>
+      <c r="H79" s="62"/>
       <c r="I79" s="59"/>
       <c r="J79" s="54">
         <v>9.3159099999999995E-2</v>
@@ -6327,11 +6322,11 @@
       <c r="S79" s="55">
         <v>613</v>
       </c>
-      <c r="T79" s="63"/>
+      <c r="T79" s="62"/>
       <c r="U79" s="55">
         <v>199</v>
       </c>
-      <c r="V79" s="63"/>
+      <c r="V79" s="62"/>
       <c r="W79" s="10"/>
       <c r="X79" s="55">
         <v>163</v>
@@ -6350,11 +6345,11 @@
       <c r="E80" s="54">
         <v>2.5430799999999998</v>
       </c>
-      <c r="F80" s="63"/>
+      <c r="F80" s="62"/>
       <c r="G80" s="54">
         <v>7.6675099999999996E-2</v>
       </c>
-      <c r="H80" s="63"/>
+      <c r="H80" s="62"/>
       <c r="I80" s="59"/>
       <c r="J80" s="54">
         <v>8.7870500000000004E-2</v>
@@ -6374,16 +6369,16 @@
       <c r="S80" s="55">
         <v>565</v>
       </c>
-      <c r="T80" s="63"/>
+      <c r="T80" s="62"/>
       <c r="U80" s="55">
         <v>72</v>
       </c>
-      <c r="V80" s="63"/>
+      <c r="V80" s="62"/>
       <c r="W80" s="10"/>
       <c r="X80" s="55">
         <v>258</v>
       </c>
-      <c r="Y80" s="62">
+      <c r="Y80" s="61">
         <v>94</v>
       </c>
     </row>
@@ -6399,11 +6394,11 @@
       <c r="E81" s="54">
         <v>3.3932699999999998</v>
       </c>
-      <c r="F81" s="63"/>
+      <c r="F81" s="62"/>
       <c r="G81" s="54">
         <v>8.8140499999999997E-2</v>
       </c>
-      <c r="H81" s="63"/>
+      <c r="H81" s="62"/>
       <c r="I81" s="59"/>
       <c r="J81" s="54">
         <v>9.5492099999999996E-2</v>

</xml_diff>

<commit_message>
Full level planning experimentation completed
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB82DC9-F293-4499-BEAC-DE92D9DC2D7E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59E7C92-924A-4291-B49F-FA8A91599DCD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -553,10 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3106,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3695,7 +3692,7 @@
         <v>163</v>
       </c>
       <c r="S18" s="9"/>
-      <c r="T18" s="42"/>
+      <c r="T18" s="9"/>
       <c r="U18" s="55">
         <v>187</v>
       </c>
@@ -3732,7 +3729,7 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
-      <c r="T19" s="42"/>
+      <c r="T19" s="9"/>
       <c r="U19" s="55">
         <v>262</v>
       </c>
@@ -3771,7 +3768,7 @@
         <v>136</v>
       </c>
       <c r="S20" s="9"/>
-      <c r="T20" s="42"/>
+      <c r="T20" s="9"/>
       <c r="U20" s="55">
         <v>364</v>
       </c>
@@ -3788,9 +3785,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="53"/>
       <c r="E21" s="59"/>
-      <c r="F21" s="54">
-        <v>260.88</v>
-      </c>
+      <c r="F21" s="59"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="59"/>
@@ -3808,9 +3803,7 @@
       <c r="Q21" s="9"/>
       <c r="R21" s="53"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="42">
-        <v>68</v>
-      </c>
+      <c r="T21" s="9"/>
       <c r="U21" s="13"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
@@ -3853,7 +3846,7 @@
         <v>98</v>
       </c>
       <c r="S22" s="9"/>
-      <c r="T22" s="42"/>
+      <c r="T22" s="9"/>
       <c r="U22" s="56"/>
       <c r="V22" s="10"/>
       <c r="W22" s="61">
@@ -3894,7 +3887,7 @@
         <v>142</v>
       </c>
       <c r="S23" s="9"/>
-      <c r="T23" s="42"/>
+      <c r="T23" s="9"/>
       <c r="U23" s="55">
         <v>241</v>
       </c>
@@ -3935,7 +3928,7 @@
         <v>93</v>
       </c>
       <c r="S24" s="9"/>
-      <c r="T24" s="42"/>
+      <c r="T24" s="9"/>
       <c r="U24" s="55">
         <v>154</v>
       </c>
@@ -3980,7 +3973,7 @@
         <v>111</v>
       </c>
       <c r="S25" s="9"/>
-      <c r="T25" s="42"/>
+      <c r="T25" s="9"/>
       <c r="U25" s="55">
         <v>199</v>
       </c>
@@ -4025,7 +4018,7 @@
         <v>106</v>
       </c>
       <c r="S26" s="9"/>
-      <c r="T26" s="42"/>
+      <c r="T26" s="9"/>
       <c r="U26" s="55">
         <v>78</v>
       </c>
@@ -4070,7 +4063,7 @@
         <v>169</v>
       </c>
       <c r="S27" s="9"/>
-      <c r="T27" s="42"/>
+      <c r="T27" s="9"/>
       <c r="U27" s="55">
         <v>187</v>
       </c>
@@ -4103,9 +4096,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="33" t="e">
         <f t="shared" si="0"/>
-        <v>260.88</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G28" s="33">
         <f t="shared" si="0"/>
@@ -4149,9 +4142,9 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="21" t="e">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" si="1"/>
@@ -4192,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="19">
         <v>8</v>
@@ -4211,7 +4204,7 @@
       </c>
       <c r="L30" s="32">
         <f>SUM(B30:K30)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M30" s="4"/>
     </row>
@@ -4367,7 +4360,7 @@
       <c r="S36" s="50">
         <v>307</v>
       </c>
-      <c r="T36" s="42"/>
+      <c r="T36" s="9"/>
       <c r="U36" s="55">
         <v>187</v>
       </c>
@@ -4412,7 +4405,7 @@
       <c r="S37" s="50">
         <v>532</v>
       </c>
-      <c r="T37" s="42"/>
+      <c r="T37" s="9"/>
       <c r="U37" s="55">
         <v>238</v>
       </c>
@@ -4457,7 +4450,7 @@
       <c r="S38" s="50">
         <v>346</v>
       </c>
-      <c r="T38" s="42"/>
+      <c r="T38" s="9"/>
       <c r="U38" s="55">
         <v>256</v>
       </c>
@@ -4502,7 +4495,7 @@
       <c r="S39" s="50">
         <v>493</v>
       </c>
-      <c r="T39" s="42"/>
+      <c r="T39" s="9"/>
       <c r="U39" s="55">
         <v>208</v>
       </c>
@@ -4547,7 +4540,7 @@
       <c r="S40" s="50">
         <v>445</v>
       </c>
-      <c r="T40" s="43"/>
+      <c r="T40" s="10"/>
       <c r="U40" s="55">
         <v>379</v>
       </c>
@@ -4592,7 +4585,7 @@
       <c r="S41" s="50">
         <v>310</v>
       </c>
-      <c r="T41" s="43"/>
+      <c r="T41" s="10"/>
       <c r="U41" s="55">
         <v>199</v>
       </c>
@@ -4637,7 +4630,7 @@
       <c r="S42" s="50">
         <v>316</v>
       </c>
-      <c r="T42" s="43"/>
+      <c r="T42" s="10"/>
       <c r="U42" s="55">
         <v>154</v>
       </c>
@@ -4682,7 +4675,7 @@
       <c r="S43" s="50">
         <v>505</v>
       </c>
-      <c r="T43" s="43"/>
+      <c r="T43" s="10"/>
       <c r="U43" s="55">
         <v>199</v>
       </c>
@@ -4729,7 +4722,7 @@
       <c r="S44" s="50">
         <v>550</v>
       </c>
-      <c r="T44" s="43"/>
+      <c r="T44" s="10"/>
       <c r="U44" s="55">
         <v>72</v>
       </c>
@@ -4776,7 +4769,7 @@
       <c r="S45" s="50">
         <v>289</v>
       </c>
-      <c r="T45" s="42"/>
+      <c r="T45" s="9"/>
       <c r="U45" s="55">
         <v>187</v>
       </c>
@@ -5054,7 +5047,7 @@
         <v>18.004999999999999</v>
       </c>
       <c r="F54" s="54">
-        <v>12.0899</v>
+        <v>11.003</v>
       </c>
       <c r="G54" s="54">
         <v>0.47940199999999999</v>
@@ -5087,7 +5080,7 @@
       <c r="S54" s="55">
         <v>355</v>
       </c>
-      <c r="T54" s="63">
+      <c r="T54" s="55">
         <v>350</v>
       </c>
       <c r="U54" s="55">
@@ -5123,7 +5116,7 @@
         <v>44.814300000000003</v>
       </c>
       <c r="F55" s="54">
-        <v>34.728400000000001</v>
+        <v>29.803100000000001</v>
       </c>
       <c r="G55" s="54">
         <v>0.38312600000000002</v>
@@ -5156,8 +5149,8 @@
       <c r="S55" s="55">
         <v>607</v>
       </c>
-      <c r="T55" s="63">
-        <v>339</v>
+      <c r="T55" s="55">
+        <v>315</v>
       </c>
       <c r="U55" s="55">
         <v>238</v>
@@ -5192,7 +5185,7 @@
         <v>19.5749</v>
       </c>
       <c r="F56" s="54">
-        <v>126.414</v>
+        <v>218.065</v>
       </c>
       <c r="G56" s="54">
         <v>0.50300400000000001</v>
@@ -5225,8 +5218,8 @@
       <c r="S56" s="55">
         <v>541</v>
       </c>
-      <c r="T56" s="63">
-        <v>671</v>
+      <c r="T56" s="55">
+        <v>790</v>
       </c>
       <c r="U56" s="55">
         <v>256</v>
@@ -5261,7 +5254,7 @@
         <v>18.940899999999999</v>
       </c>
       <c r="F57" s="54">
-        <v>1.05467</v>
+        <v>0.73758699999999999</v>
       </c>
       <c r="G57" s="54">
         <v>0.54791000000000001</v>
@@ -5294,8 +5287,8 @@
       <c r="S57" s="55">
         <v>490</v>
       </c>
-      <c r="T57" s="63">
-        <v>62</v>
+      <c r="T57" s="55">
+        <v>66</v>
       </c>
       <c r="U57" s="55">
         <v>208</v>
@@ -5361,7 +5354,7 @@
       <c r="S58" s="55">
         <v>472</v>
       </c>
-      <c r="T58" s="63"/>
+      <c r="T58" s="62"/>
       <c r="U58" s="55">
         <v>379</v>
       </c>
@@ -5395,7 +5388,7 @@
         <v>35.987299999999998</v>
       </c>
       <c r="F59" s="54">
-        <v>18.217300000000002</v>
+        <v>19.471800000000002</v>
       </c>
       <c r="G59" s="54">
         <v>0.43384499999999998</v>
@@ -5428,7 +5421,7 @@
       <c r="S59" s="55">
         <v>460</v>
       </c>
-      <c r="T59" s="63">
+      <c r="T59" s="55">
         <v>181</v>
       </c>
       <c r="U59" s="55">
@@ -5464,7 +5457,7 @@
         <v>21.556999999999999</v>
       </c>
       <c r="F60" s="54">
-        <v>1.8813</v>
+        <v>1.7900100000000001</v>
       </c>
       <c r="G60" s="54">
         <v>0.44375300000000001</v>
@@ -5497,7 +5490,7 @@
       <c r="S60" s="55">
         <v>343</v>
       </c>
-      <c r="T60" s="63">
+      <c r="T60" s="55">
         <v>120</v>
       </c>
       <c r="U60" s="55">
@@ -5533,7 +5526,7 @@
         <v>24.514700000000001</v>
       </c>
       <c r="F61" s="54">
-        <v>21.223299999999998</v>
+        <v>15.7742</v>
       </c>
       <c r="G61" s="54">
         <v>0.37591000000000002</v>
@@ -5566,7 +5559,7 @@
       <c r="S61" s="55">
         <v>526</v>
       </c>
-      <c r="T61" s="63">
+      <c r="T61" s="55">
         <v>165</v>
       </c>
       <c r="U61" s="55">
@@ -5602,7 +5595,7 @@
         <v>11.315799999999999</v>
       </c>
       <c r="F62" s="54">
-        <v>3.78572</v>
+        <v>3.8772700000000002</v>
       </c>
       <c r="G62" s="54">
         <v>0.30377300000000002</v>
@@ -5635,7 +5628,7 @@
       <c r="S62" s="55">
         <v>559</v>
       </c>
-      <c r="T62" s="63">
+      <c r="T62" s="55">
         <v>230</v>
       </c>
       <c r="U62" s="55">
@@ -5671,7 +5664,7 @@
         <v>12.3293</v>
       </c>
       <c r="F63" s="54">
-        <v>8.7304200000000005</v>
+        <v>7.0873400000000002</v>
       </c>
       <c r="G63" s="54">
         <v>0.38303500000000001</v>
@@ -5704,8 +5697,8 @@
       <c r="S63" s="55">
         <v>367</v>
       </c>
-      <c r="T63" s="63">
-        <v>208</v>
+      <c r="T63" s="55">
+        <v>146</v>
       </c>
       <c r="U63" s="55">
         <v>187</v>
@@ -5745,7 +5738,7 @@
       </c>
       <c r="F64" s="33">
         <f t="shared" si="4"/>
-        <v>25.347223333333332</v>
+        <v>34.178811888888895</v>
       </c>
       <c r="G64" s="33">
         <f t="shared" si="4"/>
@@ -5791,7 +5784,7 @@
       </c>
       <c r="F65" s="21">
         <f t="shared" si="5"/>
-        <v>37.160153806276007</v>
+        <v>65.612416276339289</v>
       </c>
       <c r="G65" s="21">
         <f t="shared" si="5"/>
@@ -5985,11 +5978,11 @@
       <c r="E72" s="54">
         <v>4.0223899999999997</v>
       </c>
-      <c r="F72" s="40"/>
+      <c r="F72" s="9"/>
       <c r="G72" s="54">
         <v>0.109879</v>
       </c>
-      <c r="H72" s="40"/>
+      <c r="H72" s="9"/>
       <c r="I72" s="59"/>
       <c r="J72" s="54">
         <v>5.3376100000000003E-2</v>
@@ -6007,11 +6000,11 @@
       <c r="S72" s="55">
         <v>364</v>
       </c>
-      <c r="T72" s="40"/>
+      <c r="T72" s="9"/>
       <c r="U72" s="55">
         <v>187</v>
       </c>
-      <c r="V72" s="40"/>
+      <c r="V72" s="9"/>
       <c r="W72" s="9"/>
       <c r="X72" s="55">
         <v>158</v>
@@ -6030,11 +6023,11 @@
       <c r="E73" s="54">
         <v>5.4539999999999997</v>
       </c>
-      <c r="F73" s="40"/>
+      <c r="F73" s="9"/>
       <c r="G73" s="54">
         <v>0.12564</v>
       </c>
-      <c r="H73" s="40"/>
+      <c r="H73" s="9"/>
       <c r="I73" s="59"/>
       <c r="J73" s="54">
         <v>0.13887099999999999</v>
@@ -6052,11 +6045,11 @@
       <c r="S73" s="55">
         <v>685</v>
       </c>
-      <c r="T73" s="40"/>
+      <c r="T73" s="9"/>
       <c r="U73" s="55">
         <v>238</v>
       </c>
-      <c r="V73" s="40"/>
+      <c r="V73" s="9"/>
       <c r="W73" s="9"/>
       <c r="X73" s="55">
         <v>208</v>
@@ -6075,11 +6068,11 @@
       <c r="E74" s="54">
         <v>5.0095099999999997</v>
       </c>
-      <c r="F74" s="40"/>
+      <c r="F74" s="9"/>
       <c r="G74" s="54">
         <v>0.16522400000000001</v>
       </c>
-      <c r="H74" s="40"/>
+      <c r="H74" s="9"/>
       <c r="I74" s="59"/>
       <c r="J74" s="54">
         <v>8.1892999999999994E-2</v>
@@ -6097,11 +6090,11 @@
       <c r="S74" s="55">
         <v>502</v>
       </c>
-      <c r="T74" s="40"/>
+      <c r="T74" s="9"/>
       <c r="U74" s="55">
         <v>256</v>
       </c>
-      <c r="V74" s="40"/>
+      <c r="V74" s="9"/>
       <c r="W74" s="9"/>
       <c r="X74" s="55">
         <v>233</v>
@@ -6120,11 +6113,11 @@
       <c r="E75" s="54">
         <v>4.3646000000000003</v>
       </c>
-      <c r="F75" s="40"/>
+      <c r="F75" s="9"/>
       <c r="G75" s="54">
         <v>0.147289</v>
       </c>
-      <c r="H75" s="40"/>
+      <c r="H75" s="9"/>
       <c r="I75" s="59"/>
       <c r="J75" s="54">
         <v>6.7930599999999994E-2</v>
@@ -6142,11 +6135,11 @@
       <c r="S75" s="55">
         <v>622</v>
       </c>
-      <c r="T75" s="40"/>
+      <c r="T75" s="9"/>
       <c r="U75" s="55">
         <v>208</v>
       </c>
-      <c r="V75" s="40"/>
+      <c r="V75" s="9"/>
       <c r="W75" s="9"/>
       <c r="X75" s="55">
         <v>158</v>
@@ -6165,11 +6158,11 @@
       <c r="E76" s="54">
         <v>4.2425199999999998</v>
       </c>
-      <c r="F76" s="62"/>
+      <c r="F76" s="10"/>
       <c r="G76" s="54">
         <v>0.19906299999999999</v>
       </c>
-      <c r="H76" s="62"/>
+      <c r="H76" s="10"/>
       <c r="I76" s="59"/>
       <c r="J76" s="54">
         <v>5.1220700000000001E-2</v>
@@ -6187,11 +6180,11 @@
       <c r="S76" s="55">
         <v>481</v>
       </c>
-      <c r="T76" s="62"/>
+      <c r="T76" s="10"/>
       <c r="U76" s="55">
         <v>379</v>
       </c>
-      <c r="V76" s="62"/>
+      <c r="V76" s="10"/>
       <c r="W76" s="10"/>
       <c r="X76" s="55">
         <v>118</v>
@@ -6210,11 +6203,11 @@
       <c r="E77" s="54">
         <v>4.8396100000000004</v>
       </c>
-      <c r="F77" s="62"/>
+      <c r="F77" s="10"/>
       <c r="G77" s="54">
         <v>0.10667500000000001</v>
       </c>
-      <c r="H77" s="62"/>
+      <c r="H77" s="10"/>
       <c r="I77" s="59"/>
       <c r="J77" s="54">
         <v>8.2027600000000006E-2</v>
@@ -6232,11 +6225,11 @@
       <c r="S77" s="55">
         <v>601</v>
       </c>
-      <c r="T77" s="62"/>
+      <c r="T77" s="10"/>
       <c r="U77" s="55">
         <v>241</v>
       </c>
-      <c r="V77" s="62"/>
+      <c r="V77" s="10"/>
       <c r="W77" s="10"/>
       <c r="X77" s="55">
         <v>148</v>
@@ -6255,11 +6248,11 @@
       <c r="E78" s="54">
         <v>3.2199</v>
       </c>
-      <c r="F78" s="62"/>
+      <c r="F78" s="10"/>
       <c r="G78" s="54">
         <v>0.106572</v>
       </c>
-      <c r="H78" s="62"/>
+      <c r="H78" s="10"/>
       <c r="I78" s="59"/>
       <c r="J78" s="54">
         <v>5.05064E-2</v>
@@ -6277,11 +6270,11 @@
       <c r="S78" s="55">
         <v>328</v>
       </c>
-      <c r="T78" s="62"/>
+      <c r="T78" s="10"/>
       <c r="U78" s="55">
         <v>154</v>
       </c>
-      <c r="V78" s="62"/>
+      <c r="V78" s="10"/>
       <c r="W78" s="10"/>
       <c r="X78" s="55">
         <v>98</v>
@@ -6300,11 +6293,11 @@
       <c r="E79" s="54">
         <v>3.1267800000000001</v>
       </c>
-      <c r="F79" s="62"/>
+      <c r="F79" s="10"/>
       <c r="G79" s="54">
         <v>8.7227299999999994E-2</v>
       </c>
-      <c r="H79" s="62"/>
+      <c r="H79" s="10"/>
       <c r="I79" s="59"/>
       <c r="J79" s="54">
         <v>9.3159099999999995E-2</v>
@@ -6322,11 +6315,11 @@
       <c r="S79" s="55">
         <v>613</v>
       </c>
-      <c r="T79" s="62"/>
+      <c r="T79" s="10"/>
       <c r="U79" s="55">
         <v>199</v>
       </c>
-      <c r="V79" s="62"/>
+      <c r="V79" s="10"/>
       <c r="W79" s="10"/>
       <c r="X79" s="55">
         <v>163</v>
@@ -6345,11 +6338,11 @@
       <c r="E80" s="54">
         <v>2.5430799999999998</v>
       </c>
-      <c r="F80" s="62"/>
+      <c r="F80" s="10"/>
       <c r="G80" s="54">
         <v>7.6675099999999996E-2</v>
       </c>
-      <c r="H80" s="62"/>
+      <c r="H80" s="10"/>
       <c r="I80" s="59"/>
       <c r="J80" s="54">
         <v>8.7870500000000004E-2</v>
@@ -6369,11 +6362,11 @@
       <c r="S80" s="55">
         <v>565</v>
       </c>
-      <c r="T80" s="62"/>
+      <c r="T80" s="10"/>
       <c r="U80" s="55">
         <v>72</v>
       </c>
-      <c r="V80" s="62"/>
+      <c r="V80" s="10"/>
       <c r="W80" s="10"/>
       <c r="X80" s="55">
         <v>258</v>
@@ -6394,11 +6387,11 @@
       <c r="E81" s="54">
         <v>3.3932699999999998</v>
       </c>
-      <c r="F81" s="62"/>
+      <c r="F81" s="9"/>
       <c r="G81" s="54">
         <v>8.8140499999999997E-2</v>
       </c>
-      <c r="H81" s="62"/>
+      <c r="H81" s="9"/>
       <c r="I81" s="59"/>
       <c r="J81" s="54">
         <v>9.5492099999999996E-2</v>
@@ -6416,11 +6409,11 @@
       <c r="S81" s="55">
         <v>370</v>
       </c>
-      <c r="T81" s="40"/>
+      <c r="T81" s="9"/>
       <c r="U81" s="55">
         <v>187</v>
       </c>
-      <c r="V81" s="40"/>
+      <c r="V81" s="9"/>
       <c r="W81" s="9"/>
       <c r="X81" s="55">
         <v>363</v>

</xml_diff>

<commit_message>
Missing indentation in agent source file
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C5DDF-79F3-40D2-9A6A-307C97BD20AD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6669C0-2705-40EF-9A2F-6566117DB85D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0" sheetId="1" r:id="rId1"/>
@@ -3230,8 +3230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236E5864-7DE8-4BC8-BF4A-4C02356587BF}">
   <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90:K99"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83:K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4253,43 +4253,43 @@
       <c r="A29" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="33">
         <f t="shared" ref="B29:K29" si="1">_xlfn.STDEV.P(B18:B27)</f>
         <v>0</v>
       </c>
-      <c r="C29" s="21" t="e">
+      <c r="C29" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="33">
         <f t="shared" si="1"/>
         <v>126.46918004003969</v>
       </c>
-      <c r="E29" s="21" t="e">
+      <c r="E29" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F29" s="21" t="e">
+      <c r="F29" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G29" s="21">
+      <c r="G29" s="33">
         <f t="shared" si="1"/>
         <v>237.16398792554915</v>
       </c>
-      <c r="H29" s="21" t="e">
+      <c r="H29" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I29" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J29" s="21">
+      <c r="J29" s="33">
         <f t="shared" si="1"/>
         <v>258.58669019735362</v>
       </c>
-      <c r="K29" s="21">
+      <c r="K29" s="33">
         <f t="shared" si="1"/>
         <v>231.23772194432291</v>
       </c>
@@ -4957,43 +4957,43 @@
       <c r="A47" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="21" t="e">
+      <c r="B47" s="33" t="e">
         <f t="shared" ref="B47:K47" si="3">_xlfn.STDEV.P(B36:B45)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C47" s="21" t="e">
+      <c r="C47" s="33" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="33">
         <f t="shared" si="3"/>
         <v>123.86685861614376</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="33">
         <f t="shared" si="3"/>
         <v>0.12216899854222542</v>
       </c>
-      <c r="F47" s="21" t="e">
+      <c r="F47" s="33" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G47" s="21">
+      <c r="G47" s="33">
         <f t="shared" si="3"/>
         <v>2.7456084754329136E-2</v>
       </c>
-      <c r="H47" s="21" t="e">
+      <c r="H47" s="33" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I47" s="21" t="e">
+      <c r="I47" s="33" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J47" s="21">
+      <c r="J47" s="33">
         <f t="shared" si="3"/>
         <v>1.8323443898197844E-2</v>
       </c>
-      <c r="K47" s="21">
+      <c r="K47" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5893,43 +5893,43 @@
       <c r="A65" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="21">
+      <c r="B65" s="33">
         <f t="shared" ref="B65:J65" si="5">_xlfn.STDEV.P(B54:B63)</f>
         <v>210.55084371985251</v>
       </c>
-      <c r="C65" s="21">
+      <c r="C65" s="33">
         <f t="shared" si="5"/>
         <v>13.842170139334407</v>
       </c>
-      <c r="D65" s="21">
+      <c r="D65" s="33">
         <f t="shared" si="5"/>
         <v>3.5680929058188222</v>
       </c>
-      <c r="E65" s="21">
+      <c r="E65" s="33">
         <f t="shared" si="5"/>
         <v>10.197231670703582</v>
       </c>
-      <c r="F65" s="21">
+      <c r="F65" s="33">
         <f t="shared" si="5"/>
         <v>65.612416276339289</v>
       </c>
-      <c r="G65" s="21">
+      <c r="G65" s="33">
         <f t="shared" si="5"/>
         <v>0.10697375139018937</v>
       </c>
-      <c r="H65" s="21">
+      <c r="H65" s="33">
         <f t="shared" si="5"/>
         <v>4.6249010564309394</v>
       </c>
-      <c r="I65" s="21">
+      <c r="I65" s="33">
         <f t="shared" si="5"/>
         <v>98.905895952484926</v>
       </c>
-      <c r="J65" s="21">
+      <c r="J65" s="33">
         <f t="shared" si="5"/>
         <v>0.57538831567365101</v>
       </c>
-      <c r="K65" s="21">
+      <c r="K65" s="33">
         <f>_xlfn.STDEV.P(K54:K63)</f>
         <v>0.28360918163998916</v>
       </c>
@@ -6597,43 +6597,43 @@
       <c r="A83" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="21" t="e">
+      <c r="B83" s="33" t="e">
         <f t="shared" ref="B83:K83" si="7">_xlfn.STDEV.P(B72:B81)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C83" s="21" t="e">
+      <c r="C83" s="33" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D83" s="21">
+      <c r="D83" s="33">
         <f t="shared" si="7"/>
         <v>0.55558893358461547</v>
       </c>
-      <c r="E83" s="21">
+      <c r="E83" s="33">
         <f t="shared" si="7"/>
         <v>0.8881203324347432</v>
       </c>
-      <c r="F83" s="21" t="e">
+      <c r="F83" s="33" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G83" s="21">
+      <c r="G83" s="33">
         <f t="shared" si="7"/>
         <v>3.6720232443094705E-2</v>
       </c>
-      <c r="H83" s="21" t="e">
+      <c r="H83" s="33" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I83" s="21" t="e">
+      <c r="I83" s="33" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J83" s="21">
+      <c r="J83" s="33">
         <f t="shared" si="7"/>
         <v>2.5496417839392639E-2</v>
       </c>
-      <c r="K83" s="21">
+      <c r="K83" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -7295,43 +7295,43 @@
       <c r="A101" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B101" s="21" t="e">
+      <c r="B101" s="33" t="e">
         <f t="shared" ref="B101:K101" si="9">_xlfn.STDEV.P(B90:B99)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C101" s="21" t="e">
+      <c r="C101" s="33" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D101" s="21">
+      <c r="D101" s="33">
         <f t="shared" si="9"/>
         <v>219.50302936757691</v>
       </c>
-      <c r="E101" s="21">
+      <c r="E101" s="33">
         <f t="shared" si="9"/>
         <v>9.914265890725364</v>
       </c>
-      <c r="F101" s="21" t="e">
+      <c r="F101" s="33" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G101" s="21">
+      <c r="G101" s="33">
         <f t="shared" si="9"/>
         <v>0.39301759637437328</v>
       </c>
-      <c r="H101" s="21" t="e">
+      <c r="H101" s="33" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I101" s="21" t="e">
+      <c r="I101" s="33" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J101" s="21">
+      <c r="J101" s="33">
         <f t="shared" si="9"/>
         <v>0.11623998861360062</v>
       </c>
-      <c r="K101" s="21" t="e">
+      <c r="K101" s="33" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -7418,8 +7418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E386126B-65E8-4C6E-8E3D-C2C060000E4B}">
   <dimension ref="A1:Z175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J120" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Z135" sqref="Z135"/>
+    <sheetView topLeftCell="J120" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M121" sqref="M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>